<commit_message>
Data visualization to check normality and initial linear regression for 2021 data
</commit_message>
<xml_diff>
--- a/data/Excel_LO_edited/Blankinship-soil-chemistry_TN-TC-OM_LO.xlsx
+++ b/data/Excel_LO_edited/Blankinship-soil-chemistry_TN-TC-OM_LO.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_email_arizona_edu/Documents/grad school/Gornish lab/Altar Valley Conservation Alliance Elkhorn-Las Delicias Demo/AVCA_ElkLD/data/Excel_LO_edited/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="34" documentId="8_{2A661D91-0D8F-472D-931E-2F6F676A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9049F380-85FE-4E01-9049-607A83819556}"/>
+  <xr:revisionPtr revIDLastSave="78" documentId="8_{2A661D91-0D8F-472D-931E-2F6F676A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E0453F7-56AB-4F3A-8C71-C0D31E0244D6}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{02775A1A-B9E6-478D-BE09-69A54B1AB19E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{02775A1A-B9E6-478D-BE09-69A54B1AB19E}"/>
   </bookViews>
   <sheets>
     <sheet name="Elise's AIR Project Spring 2022" sheetId="2" r:id="rId1"/>
     <sheet name="Loss on Ignition Luna AIR" sheetId="3" r:id="rId2"/>
-    <sheet name="soilchem_R" sheetId="1" r:id="rId3"/>
+    <sheet name="R_LO" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="212">
   <si>
     <t>Channel</t>
   </si>
@@ -661,6 +661,18 @@
   </si>
   <si>
     <t>Station 11 + 73 BAF</t>
+  </si>
+  <si>
+    <t>Baffle</t>
+  </si>
+  <si>
+    <t>One rock dam</t>
+  </si>
+  <si>
+    <t>No treatment</t>
+  </si>
+  <si>
+    <t>Station 07 + 66 BAF</t>
   </si>
 </sst>
 </file>
@@ -776,9 +788,6 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -789,14 +798,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1114,7 +1126,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B64"/>
+      <selection activeCell="C3" sqref="C3:D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1124,36 +1136,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C3">
@@ -1167,10 +1179,10 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C4">
@@ -1184,10 +1196,10 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5">
@@ -1201,10 +1213,10 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6">
@@ -1218,10 +1230,10 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -1235,10 +1247,10 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8">
@@ -1252,10 +1264,10 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C9">
@@ -1269,10 +1281,10 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C10">
@@ -1286,10 +1298,10 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C11">
@@ -1303,10 +1315,10 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C12">
@@ -1320,10 +1332,10 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>21</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C13">
@@ -1337,10 +1349,10 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C14">
@@ -1354,10 +1366,10 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C15">
@@ -1371,10 +1383,10 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>21</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C16">
@@ -1388,10 +1400,10 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>21</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C17">
@@ -1405,10 +1417,10 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>19</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C18">
@@ -1422,10 +1434,10 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C19">
@@ -1439,10 +1451,10 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C20">
@@ -1456,10 +1468,10 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C21">
@@ -1473,10 +1485,10 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C22">
@@ -1490,10 +1502,10 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C23">
@@ -1507,10 +1519,10 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>19</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C24">
@@ -1524,10 +1536,10 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>19</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C25">
@@ -1541,10 +1553,10 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>19</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C26">
@@ -1558,10 +1570,10 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>19</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C27">
@@ -1575,10 +1587,10 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>19</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C28">
@@ -1592,10 +1604,10 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>19</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C29">
@@ -1609,10 +1621,10 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>19</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C30">
@@ -1626,10 +1638,10 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>19</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C31">
@@ -1643,10 +1655,10 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>19</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C32">
@@ -1660,10 +1672,10 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>19</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C33">
@@ -1677,10 +1689,10 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>19</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C34">
@@ -1694,10 +1706,10 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>13</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C35">
@@ -1711,10 +1723,10 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>13</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C36">
@@ -1728,10 +1740,10 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>13</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C37">
@@ -1745,10 +1757,10 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>13</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C38">
@@ -1762,10 +1774,10 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>13</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C39">
@@ -1779,10 +1791,10 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>13</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C40">
@@ -1796,10 +1808,10 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>13</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C41">
@@ -1813,10 +1825,10 @@
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>13</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C42">
@@ -1830,10 +1842,10 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>13</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C43">
@@ -1847,10 +1859,10 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>13</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C44">
@@ -1864,10 +1876,10 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>13</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C45">
@@ -1881,10 +1893,10 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>13</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C46">
@@ -1898,10 +1910,10 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>13</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C47">
@@ -1915,10 +1927,10 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>13</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C48">
@@ -1932,10 +1944,10 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>13</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C49">
@@ -1949,10 +1961,10 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>13</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C50">
@@ -1966,10 +1978,10 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>12</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C51">
@@ -1983,10 +1995,10 @@
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>12</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C52">
@@ -2000,10 +2012,10 @@
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>12</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C53">
@@ -2017,10 +2029,10 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>12</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C54">
@@ -2034,10 +2046,10 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>12</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C55">
@@ -2051,10 +2063,10 @@
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>12</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C56">
@@ -2068,10 +2080,10 @@
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>12</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C57">
@@ -2085,10 +2097,10 @@
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>12</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C58">
@@ -2102,10 +2114,10 @@
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>12</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C59">
@@ -2119,10 +2131,10 @@
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>12</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C60">
@@ -2136,10 +2148,10 @@
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>12</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C61">
@@ -2153,10 +2165,10 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>12</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C62">
@@ -2170,10 +2182,10 @@
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>12</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C63">
@@ -2187,10 +2199,10 @@
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>12</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C64">
@@ -2215,8 +2227,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56470C91-933A-4BF4-A2F1-404BA9C07054}">
   <dimension ref="A1:I64"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3:I64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2233,52 +2245,52 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="5" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+      <c r="A3" s="3">
         <v>21</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C3">
@@ -2302,16 +2314,16 @@
         <f>F3-G3</f>
         <v>5.3799999999995407E-2</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="6">
         <f>(H3/F3)*100</f>
         <v>1.0725677830940077</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+      <c r="A4" s="3">
         <v>21</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C4">
@@ -2335,16 +2347,16 @@
         <f t="shared" ref="H4:H64" si="2">F4-G4</f>
         <v>5.0899999999998613E-2</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="6">
         <f t="shared" ref="I4:I64" si="3">(H4/F4)*100</f>
         <v>1.0139846209012042</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+      <c r="A5" s="3">
         <v>21</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C5">
@@ -2368,16 +2380,16 @@
         <f t="shared" si="2"/>
         <v>7.4799999999996203E-2</v>
       </c>
-      <c r="I5" s="8">
+      <c r="I5" s="6">
         <f t="shared" si="3"/>
         <v>1.4975874426891762</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+      <c r="A6" s="3">
         <v>21</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C6">
@@ -2401,16 +2413,16 @@
         <f t="shared" si="2"/>
         <v>6.0000000000002274E-2</v>
       </c>
-      <c r="I6" s="8">
+      <c r="I6" s="6">
         <f t="shared" si="3"/>
         <v>1.1940298507463143</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+      <c r="A7" s="3">
         <v>21</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C7">
@@ -2434,16 +2446,16 @@
         <f t="shared" si="2"/>
         <v>7.0700000000002206E-2</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="6">
         <f t="shared" si="3"/>
         <v>1.4036411284719206</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+      <c r="A8" s="3">
         <v>21</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8">
@@ -2467,16 +2479,16 @@
         <f t="shared" si="2"/>
         <v>5.5599999999998317E-2</v>
       </c>
-      <c r="I8" s="8">
+      <c r="I8" s="6">
         <f t="shared" si="3"/>
         <v>1.1207417859302224</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+      <c r="A9" s="3">
         <v>21</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
       <c r="C9">
@@ -2500,16 +2512,16 @@
         <f t="shared" si="2"/>
         <v>6.1700000000001864E-2</v>
       </c>
-      <c r="I9" s="8">
+      <c r="I9" s="6">
         <f t="shared" si="3"/>
         <v>1.3387432737372382</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+      <c r="A10" s="3">
         <v>21</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="C10">
@@ -2533,16 +2545,16 @@
         <f t="shared" si="2"/>
         <v>5.5599999999998317E-2</v>
       </c>
-      <c r="I10" s="8">
+      <c r="I10" s="6">
         <f t="shared" si="3"/>
         <v>1.1290257076716552</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+      <c r="A11" s="3">
         <v>21</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
       <c r="C11">
@@ -2566,16 +2578,16 @@
         <f t="shared" si="2"/>
         <v>5.6300000000000239E-2</v>
       </c>
-      <c r="I11" s="8">
+      <c r="I11" s="6">
         <f t="shared" si="3"/>
         <v>1.1150722915428846</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+      <c r="A12" s="3">
         <v>21</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="3" t="s">
         <v>31</v>
       </c>
       <c r="C12">
@@ -2599,16 +2611,16 @@
         <f t="shared" si="2"/>
         <v>5.7600000000000762E-2</v>
       </c>
-      <c r="I12" s="8">
+      <c r="I12" s="6">
         <f t="shared" si="3"/>
         <v>1.1432200698634631</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+      <c r="A13" s="3">
         <v>21</v>
       </c>
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
       <c r="C13">
@@ -2632,16 +2644,16 @@
         <f t="shared" si="2"/>
         <v>5.0300000000000011E-2</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="6">
         <f t="shared" si="3"/>
         <v>0.96404477154247226</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+      <c r="A14" s="3">
         <v>21</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
       <c r="C14">
@@ -2665,16 +2677,16 @@
         <f t="shared" si="2"/>
         <v>5.519999999999925E-2</v>
       </c>
-      <c r="I14" s="8">
+      <c r="I14" s="6">
         <f t="shared" si="3"/>
         <v>1.1088122451439102</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+      <c r="A15" s="3">
         <v>21</v>
       </c>
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
       <c r="C15">
@@ -2698,16 +2710,16 @@
         <f t="shared" si="2"/>
         <v>4.7899999999998499E-2</v>
       </c>
-      <c r="I15" s="8">
+      <c r="I15" s="6">
         <f t="shared" si="3"/>
         <v>0.96709065212999135</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+      <c r="A16" s="3">
         <v>21</v>
       </c>
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
       <c r="C16">
@@ -2731,16 +2743,16 @@
         <f t="shared" si="2"/>
         <v>4.5700000000003627E-2</v>
       </c>
-      <c r="I16" s="8">
+      <c r="I16" s="6">
         <f t="shared" si="3"/>
         <v>0.9434936102566972</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A17" s="5">
+      <c r="A17" s="4">
         <v>21</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C17">
@@ -2764,16 +2776,16 @@
         <f t="shared" si="2"/>
         <v>4.420000000000357E-2</v>
       </c>
-      <c r="I17" s="8">
+      <c r="I17" s="6">
         <f t="shared" si="3"/>
         <v>0.88497347081797073</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+      <c r="A18" s="3">
         <v>19</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
       <c r="C18">
@@ -2797,16 +2809,16 @@
         <f t="shared" si="2"/>
         <v>4.0200000000005787E-2</v>
       </c>
-      <c r="I18" s="8">
+      <c r="I18" s="6">
         <f t="shared" si="3"/>
         <v>0.81340293796296781</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+      <c r="A19" s="3">
         <v>19</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
       <c r="C19">
@@ -2830,16 +2842,16 @@
         <f t="shared" si="2"/>
         <v>7.9500000000003013E-2</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="6">
         <f t="shared" si="3"/>
         <v>1.5847702581481711</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+      <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>47</v>
       </c>
       <c r="C20">
@@ -2863,16 +2875,16 @@
         <f t="shared" si="2"/>
         <v>6.9600000000001216E-2</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="6">
         <f t="shared" si="3"/>
         <v>1.4055778823434615</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+      <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="4" t="s">
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
       <c r="C21">
@@ -2896,16 +2908,16 @@
         <f t="shared" si="2"/>
         <v>6.980000000000075E-2</v>
       </c>
-      <c r="I21" s="8">
+      <c r="I21" s="6">
         <f t="shared" si="3"/>
         <v>1.4157066363784025</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="4" t="s">
+      <c r="B22" s="3" t="s">
         <v>51</v>
       </c>
       <c r="C22">
@@ -2929,16 +2941,16 @@
         <f t="shared" si="2"/>
         <v>7.6999999999998181E-2</v>
       </c>
-      <c r="I22" s="8">
+      <c r="I22" s="6">
         <f t="shared" si="3"/>
         <v>1.5385537594660654</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+      <c r="A23" s="3">
         <v>19</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B23" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C23">
@@ -2962,16 +2974,16 @@
         <f t="shared" si="2"/>
         <v>6.6700000000004422E-2</v>
       </c>
-      <c r="I23" s="8">
+      <c r="I23" s="6">
         <f t="shared" si="3"/>
         <v>1.3870404258859685</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+      <c r="A24" s="3">
         <v>19</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B24" s="3" t="s">
         <v>55</v>
       </c>
       <c r="C24">
@@ -2995,16 +3007,16 @@
         <f t="shared" si="2"/>
         <v>6.260000000000332E-2</v>
       </c>
-      <c r="I24" s="8">
+      <c r="I24" s="6">
         <f t="shared" si="3"/>
         <v>1.2621985644004212</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+      <c r="A25" s="3">
         <v>19</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C25">
@@ -3028,16 +3040,16 @@
         <f t="shared" si="2"/>
         <v>7.2400000000001796E-2</v>
       </c>
-      <c r="I25" s="8">
+      <c r="I25" s="6">
         <f t="shared" si="3"/>
         <v>1.4547500401865001</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+      <c r="A26" s="3">
         <v>19</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C26">
@@ -3061,16 +3073,16 @@
         <f t="shared" si="2"/>
         <v>7.3799999999998533E-2</v>
       </c>
-      <c r="I26" s="8">
+      <c r="I26" s="6">
         <f t="shared" si="3"/>
         <v>1.4433231635765966</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+      <c r="A27" s="3">
         <v>19</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B27" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C27">
@@ -3094,16 +3106,16 @@
         <f t="shared" si="2"/>
         <v>5.8300000000002683E-2</v>
       </c>
-      <c r="I27" s="8">
+      <c r="I27" s="6">
         <f t="shared" si="3"/>
         <v>1.1850316076184055</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+      <c r="A28" s="3">
         <v>19</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B28" s="3" t="s">
         <v>63</v>
       </c>
       <c r="C28">
@@ -3127,16 +3139,16 @@
         <f t="shared" si="2"/>
         <v>5.3000000000004377E-2</v>
       </c>
-      <c r="I28" s="8">
+      <c r="I28" s="6">
         <f t="shared" si="3"/>
         <v>1.0571035363105965</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+      <c r="A29" s="3">
         <v>19</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C29">
@@ -3160,16 +3172,16 @@
         <f t="shared" si="2"/>
         <v>6.4299999999995805E-2</v>
       </c>
-      <c r="I29" s="8">
+      <c r="I29" s="6">
         <f t="shared" si="3"/>
         <v>1.3559965414706319</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+      <c r="A30" s="3">
         <v>19</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="B30" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C30">
@@ -3193,16 +3205,16 @@
         <f t="shared" si="2"/>
         <v>6.7099999999996385E-2</v>
       </c>
-      <c r="I30" s="8">
+      <c r="I30" s="6">
         <f t="shared" si="3"/>
         <v>1.3585746102449157</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+      <c r="A31" s="3">
         <v>19</v>
       </c>
-      <c r="B31" s="4" t="s">
+      <c r="B31" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C31">
@@ -3226,16 +3238,16 @@
         <f t="shared" si="2"/>
         <v>4.7999999999994714E-2</v>
       </c>
-      <c r="I31" s="8">
+      <c r="I31" s="6">
         <f t="shared" si="3"/>
         <v>0.96209737227144732</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+      <c r="A32" s="3">
         <v>19</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="B32" s="3" t="s">
         <v>71</v>
       </c>
       <c r="C32">
@@ -3259,16 +3271,16 @@
         <f t="shared" si="2"/>
         <v>6.0999999999999943E-2</v>
       </c>
-      <c r="I32" s="8">
+      <c r="I32" s="6">
         <f t="shared" si="3"/>
         <v>1.2182943878569996</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+      <c r="A33" s="3">
         <v>19</v>
       </c>
-      <c r="B33" s="4" t="s">
+      <c r="B33" s="3" t="s">
         <v>73</v>
       </c>
       <c r="C33">
@@ -3292,16 +3304,16 @@
         <f t="shared" si="2"/>
         <v>7.5599999999994338E-2</v>
       </c>
-      <c r="I33" s="8">
+      <c r="I33" s="6">
         <f t="shared" si="3"/>
         <v>1.5403109146104272</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>19</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C34">
@@ -3325,16 +3337,16 @@
         <f t="shared" si="2"/>
         <v>0.11489999999999867</v>
       </c>
-      <c r="I34" s="8">
+      <c r="I34" s="6">
         <f t="shared" si="3"/>
         <v>2.2696744627054115</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+      <c r="A35" s="3">
         <v>13</v>
       </c>
-      <c r="B35" s="4" t="s">
+      <c r="B35" s="3" t="s">
         <v>77</v>
       </c>
       <c r="C35">
@@ -3358,16 +3370,16 @@
         <f t="shared" si="2"/>
         <v>8.1499999999998352E-2</v>
       </c>
-      <c r="I35" s="8">
+      <c r="I35" s="6">
         <f t="shared" si="3"/>
         <v>1.6295437277561942</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+      <c r="A36" s="3">
         <v>13</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="3" t="s">
         <v>79</v>
       </c>
       <c r="C36">
@@ -3391,16 +3403,16 @@
         <f t="shared" si="2"/>
         <v>6.4799999999998192E-2</v>
       </c>
-      <c r="I36" s="8">
+      <c r="I36" s="6">
         <f t="shared" si="3"/>
         <v>1.2906052699714838</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+      <c r="A37" s="3">
         <v>13</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B37" s="3" t="s">
         <v>81</v>
       </c>
       <c r="C37">
@@ -3424,16 +3436,16 @@
         <f t="shared" si="2"/>
         <v>6.0400000000001342E-2</v>
       </c>
-      <c r="I37" s="8">
+      <c r="I37" s="6">
         <f t="shared" si="3"/>
         <v>1.1968928344959053</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+      <c r="A38" s="3">
         <v>13</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B38" s="3" t="s">
         <v>83</v>
       </c>
       <c r="C38">
@@ -3457,16 +3469,16 @@
         <f t="shared" si="2"/>
         <v>5.8600000000005537E-2</v>
       </c>
-      <c r="I38" s="8">
+      <c r="I38" s="6">
         <f t="shared" si="3"/>
         <v>1.1836470873395315</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+      <c r="A39" s="3">
         <v>13</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>85</v>
       </c>
       <c r="C39">
@@ -3490,16 +3502,16 @@
         <f t="shared" si="2"/>
         <v>6.2899999999999068E-2</v>
       </c>
-      <c r="I39" s="8">
+      <c r="I39" s="6">
         <f t="shared" si="3"/>
         <v>1.2619372442018912</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+      <c r="A40" s="3">
         <v>13</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="3" t="s">
         <v>87</v>
       </c>
       <c r="C40">
@@ -3523,16 +3535,16 @@
         <f t="shared" si="2"/>
         <v>7.260000000000133E-2</v>
       </c>
-      <c r="I40" s="8">
+      <c r="I40" s="6">
         <f t="shared" si="3"/>
         <v>1.4508683227083137</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+      <c r="A41" s="3">
         <v>13</v>
       </c>
-      <c r="B41" s="4" t="s">
+      <c r="B41" s="3" t="s">
         <v>89</v>
       </c>
       <c r="C41">
@@ -3556,16 +3568,16 @@
         <f t="shared" si="2"/>
         <v>5.5399999999998784E-2</v>
       </c>
-      <c r="I41" s="8">
+      <c r="I41" s="6">
         <f t="shared" si="3"/>
         <v>1.1063183960379985</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+      <c r="A42" s="3">
         <v>13</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B42" s="3" t="s">
         <v>91</v>
       </c>
       <c r="C42">
@@ -3589,16 +3601,16 @@
         <f t="shared" si="2"/>
         <v>5.2800000000004843E-2</v>
       </c>
-      <c r="I42" s="8">
+      <c r="I42" s="6">
         <f t="shared" si="3"/>
         <v>1.0620109821591162</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+      <c r="A43" s="3">
         <v>13</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>93</v>
       </c>
       <c r="C43">
@@ -3622,16 +3634,16 @@
         <f t="shared" si="2"/>
         <v>4.9100000000002808E-2</v>
       </c>
-      <c r="I43" s="8">
+      <c r="I43" s="6">
         <f t="shared" si="3"/>
         <v>1.0085241860943377</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+      <c r="A44" s="3">
         <v>13</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>95</v>
       </c>
       <c r="C44">
@@ -3655,16 +3667,16 @@
         <f t="shared" si="2"/>
         <v>5.8700000000001751E-2</v>
       </c>
-      <c r="I44" s="8">
+      <c r="I44" s="6">
         <f t="shared" si="3"/>
         <v>1.1914910891893342</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+      <c r="A45" s="3">
         <v>13</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>97</v>
       </c>
       <c r="C45">
@@ -3688,16 +3700,16 @@
         <f t="shared" si="2"/>
         <v>6.710000000000349E-2</v>
       </c>
-      <c r="I45" s="8">
+      <c r="I45" s="6">
         <f t="shared" si="3"/>
         <v>1.3626855669056974</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+      <c r="A46" s="3">
         <v>13</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>99</v>
       </c>
       <c r="C46">
@@ -3721,16 +3733,16 @@
         <f t="shared" si="2"/>
         <v>6.25E-2</v>
       </c>
-      <c r="I46" s="8">
+      <c r="I46" s="6">
         <f t="shared" si="3"/>
         <v>1.2781186094069528</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+      <c r="A47" s="3">
         <v>13</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>101</v>
       </c>
       <c r="C47">
@@ -3754,16 +3766,16 @@
         <f t="shared" si="2"/>
         <v>7.529999999999859E-2</v>
       </c>
-      <c r="I47" s="8">
+      <c r="I47" s="6">
         <f t="shared" si="3"/>
         <v>1.5018249267037356</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+      <c r="A48" s="3">
         <v>13</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>103</v>
       </c>
       <c r="C48">
@@ -3787,16 +3799,16 @@
         <f t="shared" si="2"/>
         <v>6.9599999999994111E-2</v>
       </c>
-      <c r="I48" s="8">
+      <c r="I48" s="6">
         <f t="shared" si="3"/>
         <v>1.3953768118846441</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+      <c r="A49" s="3">
         <v>13</v>
       </c>
-      <c r="B49" s="4" t="s">
+      <c r="B49" s="3" t="s">
         <v>105</v>
       </c>
       <c r="C49">
@@ -3820,16 +3832,16 @@
         <f t="shared" si="2"/>
         <v>5.8599999999998431E-2</v>
       </c>
-      <c r="I49" s="8">
+      <c r="I49" s="6">
         <f t="shared" si="3"/>
         <v>1.1747018141725649</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>13</v>
       </c>
-      <c r="B50" s="5" t="s">
+      <c r="B50" s="4" t="s">
         <v>107</v>
       </c>
       <c r="C50">
@@ -3853,16 +3865,16 @@
         <f t="shared" si="2"/>
         <v>5.2300000000002456E-2</v>
       </c>
-      <c r="I50" s="8">
+      <c r="I50" s="6">
         <f t="shared" si="3"/>
         <v>1.0611963314666508</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A51" s="4">
+      <c r="A51" s="3">
         <v>12</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B51" s="3" t="s">
         <v>109</v>
       </c>
       <c r="C51">
@@ -3886,16 +3898,16 @@
         <f t="shared" si="2"/>
         <v>5.9099999999993713E-2</v>
       </c>
-      <c r="I51" s="8">
+      <c r="I51" s="6">
         <f t="shared" si="3"/>
         <v>1.1858897182758199</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A52" s="4">
+      <c r="A52" s="3">
         <v>12</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B52" s="3" t="s">
         <v>111</v>
       </c>
       <c r="C52">
@@ -3919,16 +3931,16 @@
         <f t="shared" si="2"/>
         <v>4.8200000000001353E-2</v>
       </c>
-      <c r="I52" s="8">
+      <c r="I52" s="6">
         <f t="shared" si="3"/>
         <v>0.98017285205899973</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A53" s="4">
+      <c r="A53" s="3">
         <v>12</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="3" t="s">
         <v>113</v>
       </c>
       <c r="C53">
@@ -3952,16 +3964,16 @@
         <f t="shared" si="2"/>
         <v>4.9099999999995703E-2</v>
       </c>
-      <c r="I53" s="8">
+      <c r="I53" s="6">
         <f t="shared" si="3"/>
         <v>0.99173887575987663</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" s="4">
+      <c r="A54" s="3">
         <v>12</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B54" s="3" t="s">
         <v>115</v>
       </c>
       <c r="C54">
@@ -3985,16 +3997,16 @@
         <f t="shared" si="2"/>
         <v>4.8000000000001819E-2</v>
       </c>
-      <c r="I54" s="8">
+      <c r="I54" s="6">
         <f t="shared" si="3"/>
         <v>0.97505484683517096</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A55" s="4">
+      <c r="A55" s="3">
         <v>12</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B55" s="3" t="s">
         <v>117</v>
       </c>
       <c r="C55">
@@ -4018,16 +4030,16 @@
         <f t="shared" si="2"/>
         <v>5.7900000000003615E-2</v>
       </c>
-      <c r="I55" s="8">
+      <c r="I55" s="6">
         <f t="shared" si="3"/>
         <v>1.1571899670231554</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
+      <c r="A56" s="3">
         <v>12</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B56" s="3" t="s">
         <v>119</v>
       </c>
       <c r="C56">
@@ -4051,16 +4063,16 @@
         <f t="shared" si="2"/>
         <v>5.1999999999999602E-2</v>
       </c>
-      <c r="I56" s="8">
+      <c r="I56" s="6">
         <f t="shared" si="3"/>
         <v>1.0378827192527169</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A57" s="4">
+      <c r="A57" s="3">
         <v>12</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B57" s="3" t="s">
         <v>121</v>
       </c>
       <c r="C57">
@@ -4084,16 +4096,16 @@
         <f t="shared" si="2"/>
         <v>4.6600000000005082E-2</v>
       </c>
-      <c r="I57" s="8">
+      <c r="I57" s="6">
         <f t="shared" si="3"/>
         <v>0.93732400032192975</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" s="4">
+      <c r="A58" s="3">
         <v>12</v>
       </c>
-      <c r="B58" s="4" t="s">
+      <c r="B58" s="3" t="s">
         <v>123</v>
       </c>
       <c r="C58">
@@ -4117,16 +4129,16 @@
         <f t="shared" si="2"/>
         <v>4.959999999999809E-2</v>
       </c>
-      <c r="I58" s="8">
+      <c r="I58" s="6">
         <f t="shared" si="3"/>
         <v>0.99259555733436244</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A59" s="4">
+      <c r="A59" s="3">
         <v>12</v>
       </c>
-      <c r="B59" s="4" t="s">
+      <c r="B59" s="3" t="s">
         <v>125</v>
       </c>
       <c r="C59">
@@ -4150,16 +4162,16 @@
         <f t="shared" si="2"/>
         <v>4.2499999999996874E-2</v>
       </c>
-      <c r="I59" s="8">
+      <c r="I59" s="6">
         <f t="shared" si="3"/>
         <v>0.84993200543950242</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A60" s="4">
+      <c r="A60" s="3">
         <v>12</v>
       </c>
-      <c r="B60" s="4" t="s">
+      <c r="B60" s="3" t="s">
         <v>127</v>
       </c>
       <c r="C60">
@@ -4183,16 +4195,16 @@
         <f t="shared" si="2"/>
         <v>3.8399999999995771E-2</v>
       </c>
-      <c r="I60" s="8">
+      <c r="I60" s="6">
         <f t="shared" si="3"/>
         <v>0.78015481197041447</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A61" s="4">
+      <c r="A61" s="3">
         <v>12</v>
       </c>
-      <c r="B61" s="4" t="s">
+      <c r="B61" s="3" t="s">
         <v>129</v>
       </c>
       <c r="C61">
@@ -4216,16 +4228,16 @@
         <f t="shared" si="2"/>
         <v>4.0100000000002467E-2</v>
       </c>
-      <c r="I61" s="8">
+      <c r="I61" s="6">
         <f t="shared" si="3"/>
         <v>0.80383273864415705</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A62" s="4">
+      <c r="A62" s="3">
         <v>12</v>
       </c>
-      <c r="B62" s="4" t="s">
+      <c r="B62" s="3" t="s">
         <v>131</v>
       </c>
       <c r="C62">
@@ -4249,16 +4261,16 @@
         <f t="shared" si="2"/>
         <v>3.3599999999999852E-2</v>
       </c>
-      <c r="I62" s="8">
+      <c r="I62" s="6">
         <f t="shared" si="3"/>
         <v>0.67575721008808665</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A63" s="4">
+      <c r="A63" s="3">
         <v>12</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>133</v>
       </c>
       <c r="C63">
@@ -4282,16 +4294,16 @@
         <f t="shared" si="2"/>
         <v>3.3000000000001251E-2</v>
       </c>
-      <c r="I63" s="8">
+      <c r="I63" s="6">
         <f t="shared" si="3"/>
         <v>0.66775936380746725</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A64" s="4">
+      <c r="A64" s="3">
         <v>12</v>
       </c>
-      <c r="B64" s="4" t="s">
+      <c r="B64" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C64">
@@ -4315,7 +4327,7 @@
         <f t="shared" si="2"/>
         <v>3.6800000000006605E-2</v>
       </c>
-      <c r="I64" s="8">
+      <c r="I64" s="6">
         <f t="shared" si="3"/>
         <v>0.73533819562407032</v>
       </c>
@@ -4333,7 +4345,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:C16"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4341,7 +4353,7 @@
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4368,664 +4380,1429 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B2" t="s">
         <v>194</v>
       </c>
+      <c r="C2" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G2">
+        <v>1.0725677830940077</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>195</v>
       </c>
+      <c r="C3" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D3" t="s">
+        <v>209</v>
+      </c>
+      <c r="E3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.0139846209012042</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B4" t="s">
         <v>196</v>
       </c>
+      <c r="C4" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D4" t="s">
+        <v>208</v>
+      </c>
+      <c r="E4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G4">
+        <v>1.4975874426891762</v>
+      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>197</v>
       </c>
+      <c r="C5" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D5" t="s">
+        <v>208</v>
+      </c>
+      <c r="E5">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F5">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G5">
+        <v>1.1940298507463143</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>198</v>
       </c>
+      <c r="C6" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D6" t="s">
+        <v>209</v>
+      </c>
+      <c r="E6">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.193</v>
+      </c>
+      <c r="G6">
+        <v>1.4036411284719206</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
         <v>199</v>
       </c>
+      <c r="C7" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D7" t="s">
+        <v>208</v>
+      </c>
+      <c r="E7">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.128</v>
+      </c>
+      <c r="G7">
+        <v>1.1207417859302224</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>200</v>
       </c>
+      <c r="C8" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D8" t="s">
+        <v>209</v>
+      </c>
+      <c r="E8">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G8">
+        <v>1.3387432737372382</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C9" s="9">
+      <c r="B9" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C9" s="7">
         <v>44501</v>
       </c>
       <c r="D9" t="s">
-        <v>201</v>
+        <v>208</v>
+      </c>
+      <c r="E9">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F9">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="G9">
+        <v>1.1290257076716552</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" t="s">
         <v>201</v>
       </c>
+      <c r="C10" s="7">
+        <v>44501</v>
+      </c>
       <c r="D10" t="s">
-        <v>202</v>
+        <v>208</v>
+      </c>
+      <c r="E10">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="G10">
+        <v>1.1150722915428846</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
         <v>202</v>
       </c>
+      <c r="C11" s="7">
+        <v>44501</v>
+      </c>
       <c r="D11" t="s">
-        <v>203</v>
+        <v>209</v>
+      </c>
+      <c r="E11">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.08</v>
+      </c>
+      <c r="G11">
+        <v>1.1432200698634631</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B12" t="s">
         <v>203</v>
       </c>
+      <c r="C12" s="7">
+        <v>44501</v>
+      </c>
       <c r="D12" t="s">
-        <v>204</v>
+        <v>208</v>
+      </c>
+      <c r="E12">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F12">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="G12">
+        <v>0.96404477154247226</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B13" t="s">
         <v>204</v>
       </c>
+      <c r="C13" s="7">
+        <v>44501</v>
+      </c>
       <c r="D13" t="s">
-        <v>205</v>
+        <v>209</v>
+      </c>
+      <c r="E13">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F13">
+        <v>0.151</v>
+      </c>
+      <c r="G13">
+        <v>1.1088122451439102</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
         <v>205</v>
       </c>
+      <c r="C14" s="7">
+        <v>44501</v>
+      </c>
       <c r="D14" t="s">
-        <v>206</v>
+        <v>208</v>
+      </c>
+      <c r="E14">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F14">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G14">
+        <v>0.96709065212999135</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B15" t="s">
         <v>206</v>
       </c>
+      <c r="C15" s="7">
+        <v>44501</v>
+      </c>
       <c r="D15" t="s">
-        <v>207</v>
+        <v>209</v>
+      </c>
+      <c r="E15">
+        <v>1.4E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.104</v>
+      </c>
+      <c r="G15">
+        <v>0.9434936102566972</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
+      <c r="C16" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D16" t="s">
+        <v>208</v>
+      </c>
+      <c r="E16">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F16">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="G16">
+        <v>0.88497347081797073</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B17" t="s">
         <v>177</v>
       </c>
-      <c r="C17" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
+      <c r="C17" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D17" t="s">
+        <v>210</v>
+      </c>
+      <c r="E17">
+        <v>0.01</v>
+      </c>
+      <c r="F17">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="G17">
+        <v>0.81340293796296781</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B18" t="s">
         <v>178</v>
       </c>
-      <c r="C18" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D18" t="s">
+        <v>210</v>
+      </c>
+      <c r="E18">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F18">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G18">
+        <v>1.5847702581481711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B19" t="s">
         <v>179</v>
       </c>
-      <c r="C19" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
+      <c r="C19" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D19" t="s">
+        <v>210</v>
+      </c>
+      <c r="E19">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G19">
+        <v>1.4055778823434615</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B20" t="s">
         <v>180</v>
       </c>
-      <c r="C20" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="4" t="s">
+      <c r="C20" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D20" t="s">
+        <v>210</v>
+      </c>
+      <c r="E20">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.125</v>
+      </c>
+      <c r="G20">
+        <v>1.4157066363784025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B21" t="s">
         <v>181</v>
       </c>
-      <c r="C21" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
+      <c r="C21" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D21" t="s">
+        <v>210</v>
+      </c>
+      <c r="E21">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.152</v>
+      </c>
+      <c r="G21">
+        <v>1.5385537594660654</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B22" t="s">
         <v>182</v>
       </c>
-      <c r="C22" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
+      <c r="C22" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D22" t="s">
+        <v>210</v>
+      </c>
+      <c r="E22">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F22">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="G22">
+        <v>1.3870404258859685</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B23" t="s">
         <v>183</v>
       </c>
-      <c r="C23" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
+      <c r="C23" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D23" t="s">
+        <v>210</v>
+      </c>
+      <c r="E23">
+        <v>0.01</v>
+      </c>
+      <c r="F23">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="G23">
+        <v>1.2621985644004212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B24" t="s">
         <v>184</v>
       </c>
-      <c r="C24" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="C24" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D24" t="s">
+        <v>210</v>
+      </c>
+      <c r="E24">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="G24">
+        <v>1.4547500401865001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B25" t="s">
         <v>185</v>
       </c>
-      <c r="C25" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+      <c r="C25" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D25" t="s">
+        <v>210</v>
+      </c>
+      <c r="E25">
+        <v>1.9E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G25">
+        <v>1.4433231635765966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B26" t="s">
         <v>186</v>
       </c>
-      <c r="C26" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="4" t="s">
+      <c r="C26" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D26" t="s">
+        <v>210</v>
+      </c>
+      <c r="E26">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="G26">
+        <v>1.1850316076184055</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B27" t="s">
         <v>187</v>
       </c>
-      <c r="C27" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="4" t="s">
+      <c r="C27" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D27" t="s">
+        <v>210</v>
+      </c>
+      <c r="E27">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F27">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="G27">
+        <v>1.0571035363105965</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B28" t="s">
         <v>188</v>
       </c>
-      <c r="C28" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="4" t="s">
+      <c r="C28" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D28" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G28">
+        <v>1.3559965414706319</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B29" t="s">
         <v>189</v>
       </c>
-      <c r="C29" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="4" t="s">
+      <c r="C29" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D29" t="s">
+        <v>210</v>
+      </c>
+      <c r="E29">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.157</v>
+      </c>
+      <c r="G29">
+        <v>1.3585746102449157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B30" t="s">
         <v>190</v>
       </c>
-      <c r="C30" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="4" t="s">
+      <c r="C30" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D30" t="s">
+        <v>210</v>
+      </c>
+      <c r="E30">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F30">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G30">
+        <v>0.96209737227144732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B31" t="s">
         <v>191</v>
       </c>
-      <c r="C31" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="4" t="s">
+      <c r="C31" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D31" t="s">
+        <v>210</v>
+      </c>
+      <c r="E31">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="F31">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="G31">
+        <v>1.2182943878569996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B32" t="s">
         <v>192</v>
       </c>
-      <c r="C32" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="4" t="s">
+      <c r="C32" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D32" t="s">
+        <v>210</v>
+      </c>
+      <c r="E32">
+        <v>3.9E-2</v>
+      </c>
+      <c r="F32">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="G32">
+        <v>1.5403109146104272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>144</v>
       </c>
       <c r="B33" t="s">
         <v>193</v>
       </c>
-      <c r="C33" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="4" t="s">
+      <c r="C33" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D33" t="s">
+        <v>210</v>
+      </c>
+      <c r="E33">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.73</v>
+      </c>
+      <c r="G33">
+        <v>2.2696744627054115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B34" t="s">
         <v>161</v>
       </c>
-      <c r="C34" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A35" s="4" t="s">
+      <c r="C34" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D34" t="s">
+        <v>208</v>
+      </c>
+      <c r="E34">
+        <v>0.02</v>
+      </c>
+      <c r="F34">
+        <v>0.182</v>
+      </c>
+      <c r="G34">
+        <v>1.6295437277561942</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B35" t="s">
         <v>162</v>
       </c>
-      <c r="C35" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
+      <c r="C35" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D35" t="s">
+        <v>209</v>
+      </c>
+      <c r="E35">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.08</v>
+      </c>
+      <c r="G35">
+        <v>1.2906052699714838</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B36" t="s">
         <v>163</v>
       </c>
-      <c r="C36" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A37" s="4" t="s">
+      <c r="C36" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D36" t="s">
+        <v>208</v>
+      </c>
+      <c r="E36">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F36">
+        <v>5.5E-2</v>
+      </c>
+      <c r="G36">
+        <v>1.1968928344959053</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B37" t="s">
         <v>164</v>
       </c>
-      <c r="C37" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A38" s="4" t="s">
+      <c r="C37" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D37" t="s">
+        <v>209</v>
+      </c>
+      <c r="E37">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F37">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="G37">
+        <v>1.1836470873395315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B38" t="s">
         <v>165</v>
       </c>
-      <c r="C38" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A39" s="4" t="s">
+      <c r="C38" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D38" t="s">
+        <v>209</v>
+      </c>
+      <c r="E38">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.129</v>
+      </c>
+      <c r="G38">
+        <v>1.2619372442018912</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B39" t="s">
         <v>166</v>
       </c>
-      <c r="C39" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
+      <c r="C39" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D39" t="s">
+        <v>208</v>
+      </c>
+      <c r="E39">
+        <v>0.02</v>
+      </c>
+      <c r="F39">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="G39">
+        <v>1.4508683227083137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B40" t="s">
         <v>167</v>
       </c>
-      <c r="C40" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="4" t="s">
+      <c r="C40" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D40" t="s">
+        <v>209</v>
+      </c>
+      <c r="E40">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F40">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="G40">
+        <v>1.1063183960379985</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B41" t="s">
         <v>168</v>
       </c>
-      <c r="C41" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="4" t="s">
+      <c r="C41" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D41" t="s">
+        <v>208</v>
+      </c>
+      <c r="E41">
+        <v>0.01</v>
+      </c>
+      <c r="F41">
+        <v>0.06</v>
+      </c>
+      <c r="G41">
+        <v>1.0620109821591162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B42" t="s">
         <v>169</v>
       </c>
-      <c r="C42" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
+      <c r="C42" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D42" t="s">
+        <v>209</v>
+      </c>
+      <c r="E42">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F42">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="G42">
+        <v>1.0085241860943377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B43" t="s">
         <v>170</v>
       </c>
-      <c r="C43" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="4" t="s">
+      <c r="C43" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D43" t="s">
+        <v>208</v>
+      </c>
+      <c r="E43">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F43">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G43">
+        <v>1.1914910891893342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B44" t="s">
         <v>171</v>
       </c>
-      <c r="C44" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="4" t="s">
+      <c r="C44" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D44" t="s">
+        <v>209</v>
+      </c>
+      <c r="E44">
+        <v>2.4E-2</v>
+      </c>
+      <c r="F44">
+        <v>0.24299999999999999</v>
+      </c>
+      <c r="G44">
+        <v>1.3626855669056974</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B45" t="s">
         <v>172</v>
       </c>
-      <c r="C45" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="4" t="s">
+      <c r="C45" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E45">
+        <v>2.3E-2</v>
+      </c>
+      <c r="F45">
+        <v>0.193</v>
+      </c>
+      <c r="G45">
+        <v>1.2781186094069528</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B46" t="s">
         <v>173</v>
       </c>
-      <c r="C46" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="4" t="s">
+      <c r="C46" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D46" t="s">
+        <v>208</v>
+      </c>
+      <c r="E46">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F46">
+        <v>0.32900000000000001</v>
+      </c>
+      <c r="G46">
+        <v>1.5018249267037356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B47" t="s">
         <v>174</v>
       </c>
-      <c r="C47" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="4" t="s">
+      <c r="C47" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D47" t="s">
+        <v>209</v>
+      </c>
+      <c r="E47">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="F47">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G47">
+        <v>1.3953768118846441</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B48" t="s">
         <v>175</v>
       </c>
-      <c r="C48" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="4" t="s">
+      <c r="C48" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D48" t="s">
+        <v>208</v>
+      </c>
+      <c r="E48">
+        <v>0.02</v>
+      </c>
+      <c r="F48">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="G48">
+        <v>1.1747018141725649</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
         <v>145</v>
       </c>
       <c r="B49" t="s">
         <v>176</v>
       </c>
-      <c r="C49" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="4" t="s">
+      <c r="C49" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D49" t="s">
+        <v>209</v>
+      </c>
+      <c r="E49">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F49">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G49">
+        <v>1.0611963314666508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B50" t="s">
         <v>147</v>
       </c>
-      <c r="C50" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="4" t="s">
+      <c r="C50" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D50" t="s">
+        <v>210</v>
+      </c>
+      <c r="E50">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="F50">
+        <v>0.15</v>
+      </c>
+      <c r="G50">
+        <v>1.1858897182758199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B51" t="s">
         <v>148</v>
       </c>
-      <c r="C51" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A52" s="4" t="s">
+      <c r="C51" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D51" t="s">
+        <v>210</v>
+      </c>
+      <c r="E51">
+        <v>0.01</v>
+      </c>
+      <c r="F51">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="G51">
+        <v>0.98017285205899973</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B52" t="s">
         <v>149</v>
       </c>
-      <c r="C52" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A53" s="4" t="s">
+      <c r="C52" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D52" t="s">
+        <v>210</v>
+      </c>
+      <c r="E52">
+        <v>0.01</v>
+      </c>
+      <c r="F52">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="G52">
+        <v>0.99173887575987663</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B53" t="s">
         <v>150</v>
       </c>
-      <c r="C53" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A54" s="4" t="s">
+      <c r="C53" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D53" t="s">
+        <v>210</v>
+      </c>
+      <c r="E53">
+        <v>0.01</v>
+      </c>
+      <c r="F53">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="G53">
+        <v>0.97505484683517096</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B54" t="s">
         <v>151</v>
       </c>
-      <c r="C54" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A55" s="4" t="s">
+      <c r="C54" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D54" t="s">
+        <v>210</v>
+      </c>
+      <c r="E54">
+        <v>1.6E-2</v>
+      </c>
+      <c r="F54">
+        <v>0.127</v>
+      </c>
+      <c r="G54">
+        <v>1.1571899670231554</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B55" t="s">
         <v>152</v>
       </c>
-      <c r="C55" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A56" s="4" t="s">
+      <c r="C55" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D55" t="s">
+        <v>210</v>
+      </c>
+      <c r="E55">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F55">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="G55">
+        <v>1.0378827192527169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B56" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A57" s="4" t="s">
+      <c r="C56" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D56" t="s">
+        <v>210</v>
+      </c>
+      <c r="E56">
+        <v>0.01</v>
+      </c>
+      <c r="F56">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G56">
+        <v>0.93732400032192975</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B57" t="s">
         <v>154</v>
       </c>
-      <c r="C57" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A58" s="4" t="s">
+      <c r="C57" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D57" t="s">
+        <v>210</v>
+      </c>
+      <c r="E57">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F57">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="G57">
+        <v>0.99259555733436244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B58" t="s">
         <v>155</v>
       </c>
-      <c r="C58" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A59" s="4" t="s">
+      <c r="C58" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D58" t="s">
+        <v>210</v>
+      </c>
+      <c r="E58">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="F58">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="G58">
+        <v>0.84993200543950242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B59" t="s">
         <v>156</v>
       </c>
-      <c r="C59" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A60" s="4" t="s">
+      <c r="C59" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D59" t="s">
+        <v>210</v>
+      </c>
+      <c r="E59">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F59">
+        <v>0.05</v>
+      </c>
+      <c r="G59">
+        <v>0.78015481197041447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B60" t="s">
         <v>157</v>
       </c>
-      <c r="C60" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A61" s="4" t="s">
+      <c r="C60" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D60" t="s">
+        <v>210</v>
+      </c>
+      <c r="E60">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="F60">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G60">
+        <v>0.80383273864415705</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B61" t="s">
         <v>158</v>
       </c>
-      <c r="C61" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A62" s="4" t="s">
+      <c r="C61" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D61" t="s">
+        <v>210</v>
+      </c>
+      <c r="E61">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="F61">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="G61">
+        <v>0.67575721008808665</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B62" t="s">
         <v>159</v>
       </c>
-      <c r="C62" s="9">
-        <v>44501</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A63" s="4" t="s">
+      <c r="C62" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D62" t="s">
+        <v>210</v>
+      </c>
+      <c r="E62">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F62">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="G62">
+        <v>0.66775936380746725</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>146</v>
       </c>
       <c r="B63" t="s">
         <v>160</v>
       </c>
-      <c r="C63" s="9">
-        <v>44501</v>
+      <c r="C63" s="7">
+        <v>44501</v>
+      </c>
+      <c r="D63" t="s">
+        <v>210</v>
+      </c>
+      <c r="E63">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="F63">
+        <v>0.105</v>
+      </c>
+      <c r="G63">
+        <v>0.73533819562407032</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Treatment from Blankinship spreadsheet
</commit_message>
<xml_diff>
--- a/data/Excel_LO_edited/Blankinship-soil-chemistry_TN-TC-OM_LO.xlsx
+++ b/data/Excel_LO_edited/Blankinship-soil-chemistry_TN-TC-OM_LO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_email_arizona_edu/Documents/grad school/Gornish lab/Altar Valley Conservation Alliance Elkhorn-Las Delicias Demo/AVCA_ElkLD/data/Excel_LO_edited/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/02_AVCA Elkhorn-Las Delicias/AVCA_ElkLD/data/Excel_LO_edited/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="78" documentId="8_{2A661D91-0D8F-472D-931E-2F6F676A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E0453F7-56AB-4F3A-8C71-C0D31E0244D6}"/>
+  <xr:revisionPtr revIDLastSave="81" documentId="8_{2A661D91-0D8F-472D-931E-2F6F676A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5D0CEFE-EE77-4243-B63F-942AE3E3EB3B}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{02775A1A-B9E6-478D-BE09-69A54B1AB19E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{02775A1A-B9E6-478D-BE09-69A54B1AB19E}"/>
   </bookViews>
   <sheets>
     <sheet name="Elise's AIR Project Spring 2022" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="213">
   <si>
     <t>Channel</t>
   </si>
@@ -673,6 +673,9 @@
   </si>
   <si>
     <t>Station 07 + 66 BAF</t>
+  </si>
+  <si>
+    <t>Upland treatment</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1118,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4345,7 +4348,7 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D17" sqref="D17:D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4353,7 +4356,7 @@
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
     <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -4735,7 +4738,7 @@
         <v>44501</v>
       </c>
       <c r="D17" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E17">
         <v>0.01</v>
@@ -4758,7 +4761,7 @@
         <v>44501</v>
       </c>
       <c r="D18" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E18">
         <v>1.7999999999999999E-2</v>
@@ -4781,7 +4784,7 @@
         <v>44501</v>
       </c>
       <c r="D19" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E19">
         <v>1.0999999999999999E-2</v>
@@ -4804,7 +4807,7 @@
         <v>44501</v>
       </c>
       <c r="D20" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E20">
         <v>1.7000000000000001E-2</v>
@@ -4827,7 +4830,7 @@
         <v>44501</v>
       </c>
       <c r="D21" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E21">
         <v>1.7999999999999999E-2</v>
@@ -4850,7 +4853,7 @@
         <v>44501</v>
       </c>
       <c r="D22" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E22">
         <v>1.4999999999999999E-2</v>
@@ -4873,7 +4876,7 @@
         <v>44501</v>
       </c>
       <c r="D23" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E23">
         <v>0.01</v>
@@ -4896,7 +4899,7 @@
         <v>44501</v>
       </c>
       <c r="D24" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E24">
         <v>1.7999999999999999E-2</v>
@@ -4919,7 +4922,7 @@
         <v>44501</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E25">
         <v>1.9E-2</v>
@@ -4942,7 +4945,7 @@
         <v>44501</v>
       </c>
       <c r="D26" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E26">
         <v>1.4999999999999999E-2</v>
@@ -4965,7 +4968,7 @@
         <v>44501</v>
       </c>
       <c r="D27" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E27">
         <v>1.2999999999999999E-2</v>
@@ -4988,7 +4991,7 @@
         <v>44501</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E28">
         <v>2.5000000000000001E-2</v>
@@ -5011,7 +5014,7 @@
         <v>44501</v>
       </c>
       <c r="D29" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E29">
         <v>2.1000000000000001E-2</v>
@@ -5034,7 +5037,7 @@
         <v>44501</v>
       </c>
       <c r="D30" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E30">
         <v>1.0999999999999999E-2</v>
@@ -5057,7 +5060,7 @@
         <v>44501</v>
       </c>
       <c r="D31" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E31">
         <v>2.5000000000000001E-2</v>
@@ -5080,7 +5083,7 @@
         <v>44501</v>
       </c>
       <c r="D32" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E32">
         <v>3.9E-2</v>
@@ -5103,7 +5106,7 @@
         <v>44501</v>
       </c>
       <c r="D33" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="E33">
         <v>6.6000000000000003E-2</v>

</xml_diff>

<commit_message>
Add all relevant 2021 variables, and screen for normality, and compile clean data
</commit_message>
<xml_diff>
--- a/data/Excel_LO_edited/Blankinship-soil-chemistry_TN-TC-OM_LO.xlsx
+++ b/data/Excel_LO_edited/Blankinship-soil-chemistry_TN-TC-OM_LO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26501"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailarizona-my.sharepoint.com/personal/lossanna_arizona_edu/Documents/grad school/Gornish lab/02_AVCA Elkhorn-Las Delicias/AVCA_ElkLD/data/Excel_LO_edited/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{2A661D91-0D8F-472D-931E-2F6F676A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5D0CEFE-EE77-4243-B63F-942AE3E3EB3B}"/>
+  <xr:revisionPtr revIDLastSave="98" documentId="8_{2A661D91-0D8F-472D-931E-2F6F676A2761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF234349-805E-416E-A924-9784AB4DBA97}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15270" activeTab="2" xr2:uid="{02775A1A-B9E6-478D-BE09-69A54B1AB19E}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{02775A1A-B9E6-478D-BE09-69A54B1AB19E}"/>
   </bookViews>
   <sheets>
     <sheet name="Elise's AIR Project Spring 2022" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="210">
   <si>
     <t>Channel</t>
   </si>
@@ -45,12 +45,6 @@
     <t>Station</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Treatment</t>
-  </si>
-  <si>
     <t>TN_perc</t>
   </si>
   <si>
@@ -663,19 +657,16 @@
     <t>Station 11 + 73 BAF</t>
   </si>
   <si>
-    <t>Baffle</t>
-  </si>
-  <si>
-    <t>One rock dam</t>
-  </si>
-  <si>
-    <t>No treatment</t>
-  </si>
-  <si>
     <t>Station 07 + 66 BAF</t>
   </si>
   <si>
-    <t>Upland treatment</t>
+    <t>Treated</t>
+  </si>
+  <si>
+    <t>Treatment3</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -789,7 +780,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -805,7 +796,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1118,7 +1108,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1139,29 +1129,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
+      <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -1169,7 +1159,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>1.0999999999999999E-2</v>
@@ -1178,7 +1168,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
@@ -1186,7 +1176,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>1.2999999999999999E-2</v>
@@ -1195,7 +1185,7 @@
         <v>6.4000000000000001E-2</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -1203,7 +1193,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>2.1999999999999999E-2</v>
@@ -1212,7 +1202,7 @@
         <v>0.18099999999999999</v>
       </c>
       <c r="E5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
@@ -1220,7 +1210,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>1.4999999999999999E-2</v>
@@ -1229,7 +1219,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -1237,7 +1227,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>2.1000000000000001E-2</v>
@@ -1246,7 +1236,7 @@
         <v>0.193</v>
       </c>
       <c r="E7" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -1254,7 +1244,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>1.7999999999999999E-2</v>
@@ -1263,7 +1253,7 @@
         <v>0.128</v>
       </c>
       <c r="E8" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -1271,7 +1261,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>2.1000000000000001E-2</v>
@@ -1280,7 +1270,7 @@
         <v>0.19400000000000001</v>
       </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -1288,7 +1278,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>1.2E-2</v>
@@ -1297,7 +1287,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="E10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -1305,7 +1295,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>1.0999999999999999E-2</v>
@@ -1314,7 +1304,7 @@
         <v>8.1000000000000003E-2</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -1322,7 +1312,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>1.4E-2</v>
@@ -1331,7 +1321,7 @@
         <v>0.08</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -1339,7 +1329,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>1.2999999999999999E-2</v>
@@ -1348,7 +1338,7 @@
         <v>7.4999999999999997E-2</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -1356,7 +1346,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>1.4E-2</v>
@@ -1365,7 +1355,7 @@
         <v>0.151</v>
       </c>
       <c r="E14" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -1373,7 +1363,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>1.2999999999999999E-2</v>
@@ -1382,7 +1372,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="E15" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -1390,7 +1380,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>1.4E-2</v>
@@ -1399,7 +1389,7 @@
         <v>0.104</v>
       </c>
       <c r="E16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -1407,7 +1397,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>1.6E-2</v>
@@ -1416,7 +1406,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="E17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -1424,7 +1414,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18">
         <v>0.01</v>
@@ -1433,7 +1423,7 @@
         <v>5.2999999999999999E-2</v>
       </c>
       <c r="E18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -1441,7 +1431,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>1.7999999999999999E-2</v>
@@ -1450,7 +1440,7 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="E19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -1458,7 +1448,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>1.0999999999999999E-2</v>
@@ -1467,7 +1457,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="E20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -1475,7 +1465,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>1.7000000000000001E-2</v>
@@ -1484,7 +1474,7 @@
         <v>0.125</v>
       </c>
       <c r="E21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -1492,7 +1482,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22">
         <v>1.7999999999999999E-2</v>
@@ -1501,7 +1491,7 @@
         <v>0.152</v>
       </c>
       <c r="E22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -1509,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23">
         <v>1.4999999999999999E-2</v>
@@ -1518,7 +1508,7 @@
         <v>8.4000000000000005E-2</v>
       </c>
       <c r="E23" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -1526,7 +1516,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24">
         <v>0.01</v>
@@ -1535,7 +1525,7 @@
         <v>4.8000000000000001E-2</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -1543,7 +1533,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>1.7999999999999999E-2</v>
@@ -1552,7 +1542,7 @@
         <v>0.18099999999999999</v>
       </c>
       <c r="E25" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -1560,7 +1550,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26">
         <v>1.9E-2</v>
@@ -1569,7 +1559,7 @@
         <v>0.14099999999999999</v>
       </c>
       <c r="E26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -1577,7 +1567,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27">
         <v>1.4999999999999999E-2</v>
@@ -1586,7 +1576,7 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="E27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -1594,7 +1584,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <v>1.2999999999999999E-2</v>
@@ -1603,7 +1593,7 @@
         <v>6.9000000000000006E-2</v>
       </c>
       <c r="E28" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -1611,7 +1601,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29">
         <v>2.5000000000000001E-2</v>
@@ -1620,7 +1610,7 @@
         <v>0.24099999999999999</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -1628,7 +1618,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30">
         <v>2.1000000000000001E-2</v>
@@ -1637,7 +1627,7 @@
         <v>0.157</v>
       </c>
       <c r="E30" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -1645,7 +1635,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31">
         <v>1.0999999999999999E-2</v>
@@ -1654,7 +1644,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="E31" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -1662,7 +1652,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32">
         <v>2.5000000000000001E-2</v>
@@ -1671,7 +1661,7 @@
         <v>0.20499999999999999</v>
       </c>
       <c r="E32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
@@ -1679,7 +1669,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33">
         <v>3.9E-2</v>
@@ -1688,7 +1678,7 @@
         <v>0.40699999999999997</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.3">
@@ -1696,7 +1686,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34">
         <v>6.6000000000000003E-2</v>
@@ -1705,7 +1695,7 @@
         <v>0.73</v>
       </c>
       <c r="E34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.3">
@@ -1713,7 +1703,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <v>0.02</v>
@@ -1722,7 +1712,7 @@
         <v>0.182</v>
       </c>
       <c r="E35" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.3">
@@ -1730,7 +1720,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>1.2E-2</v>
@@ -1739,7 +1729,7 @@
         <v>0.08</v>
       </c>
       <c r="E36" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.3">
@@ -1747,7 +1737,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C37">
         <v>1.2E-2</v>
@@ -1756,7 +1746,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
@@ -1764,7 +1754,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38">
         <v>1.0999999999999999E-2</v>
@@ -1773,7 +1763,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="E38" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.3">
@@ -1781,7 +1771,7 @@
         <v>13</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39">
         <v>1.7000000000000001E-2</v>
@@ -1790,7 +1780,7 @@
         <v>0.129</v>
       </c>
       <c r="E39" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.3">
@@ -1798,7 +1788,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40">
         <v>0.02</v>
@@ -1807,7 +1797,7 @@
         <v>0.17100000000000001</v>
       </c>
       <c r="E40" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.3">
@@ -1815,7 +1805,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41">
         <v>1.2E-2</v>
@@ -1824,7 +1814,7 @@
         <v>5.6000000000000001E-2</v>
       </c>
       <c r="E41" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.3">
@@ -1832,7 +1822,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42">
         <v>0.01</v>
@@ -1841,7 +1831,7 @@
         <v>0.06</v>
       </c>
       <c r="E42" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.3">
@@ -1849,7 +1839,7 @@
         <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43">
         <v>8.0000000000000002E-3</v>
@@ -1858,7 +1848,7 @@
         <v>5.8999999999999997E-2</v>
       </c>
       <c r="E43" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.3">
@@ -1866,7 +1856,7 @@
         <v>13</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C44">
         <v>1.7999999999999999E-2</v>
@@ -1875,7 +1865,7 @@
         <v>0.13300000000000001</v>
       </c>
       <c r="E44" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.3">
@@ -1883,7 +1873,7 @@
         <v>13</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45">
         <v>2.4E-2</v>
@@ -1892,7 +1882,7 @@
         <v>0.24299999999999999</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.3">
@@ -1900,7 +1890,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46">
         <v>2.3E-2</v>
@@ -1909,7 +1899,7 @@
         <v>0.193</v>
       </c>
       <c r="E46" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.3">
@@ -1917,7 +1907,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47">
         <v>3.2000000000000001E-2</v>
@@ -1926,7 +1916,7 @@
         <v>0.32900000000000001</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.3">
@@ -1934,7 +1924,7 @@
         <v>13</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C48">
         <v>2.9000000000000001E-2</v>
@@ -1943,7 +1933,7 @@
         <v>0.28299999999999997</v>
       </c>
       <c r="E48" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.3">
@@ -1951,7 +1941,7 @@
         <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C49">
         <v>0.02</v>
@@ -1960,7 +1950,7 @@
         <v>0.16800000000000001</v>
       </c>
       <c r="E49" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.3">
@@ -1968,7 +1958,7 @@
         <v>13</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C50">
         <v>1.4999999999999999E-2</v>
@@ -1977,7 +1967,7 @@
         <v>9.5000000000000001E-2</v>
       </c>
       <c r="E50" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.3">
@@ -1985,7 +1975,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C51">
         <v>1.7999999999999999E-2</v>
@@ -1994,7 +1984,7 @@
         <v>0.15</v>
       </c>
       <c r="E51" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.3">
@@ -2002,7 +1992,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C52">
         <v>0.01</v>
@@ -2011,7 +2001,7 @@
         <v>5.1999999999999998E-2</v>
       </c>
       <c r="E52" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.3">
@@ -2019,7 +2009,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C53">
         <v>0.01</v>
@@ -2028,7 +2018,7 @@
         <v>8.3000000000000004E-2</v>
       </c>
       <c r="E53" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.3">
@@ -2036,7 +2026,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C54">
         <v>0.01</v>
@@ -2045,7 +2035,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="E54" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.3">
@@ -2053,7 +2043,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C55">
         <v>1.6E-2</v>
@@ -2062,7 +2052,7 @@
         <v>0.127</v>
       </c>
       <c r="E55" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.3">
@@ -2070,7 +2060,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C56">
         <v>1.0999999999999999E-2</v>
@@ -2079,7 +2069,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="E56" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.3">
@@ -2087,7 +2077,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C57">
         <v>0.01</v>
@@ -2096,7 +2086,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="E57" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.3">
@@ -2104,7 +2094,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C58">
         <v>1.2E-2</v>
@@ -2113,7 +2103,7 @@
         <v>7.3999999999999996E-2</v>
       </c>
       <c r="E58" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.3">
@@ -2121,7 +2111,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C59">
         <v>1.2999999999999999E-2</v>
@@ -2130,7 +2120,7 @@
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="E59" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.3">
@@ -2138,7 +2128,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C60">
         <v>8.9999999999999993E-3</v>
@@ -2147,7 +2137,7 @@
         <v>0.05</v>
       </c>
       <c r="E60" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -2155,7 +2145,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C61">
         <v>1.0999999999999999E-2</v>
@@ -2164,7 +2154,7 @@
         <v>5.0999999999999997E-2</v>
       </c>
       <c r="E61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
@@ -2172,7 +2162,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C62">
         <v>8.9999999999999993E-3</v>
@@ -2181,7 +2171,7 @@
         <v>4.2999999999999997E-2</v>
       </c>
       <c r="E62" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
@@ -2189,7 +2179,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C63">
         <v>8.0000000000000002E-3</v>
@@ -2198,7 +2188,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E63" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
@@ -2206,7 +2196,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C64">
         <v>1.4999999999999999E-2</v>
@@ -2215,7 +2205,7 @@
         <v>0.105</v>
       </c>
       <c r="E64" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2248,45 +2238,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="A1" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
     </row>
     <row r="2" spans="1:9" ht="31.2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>141</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
@@ -2294,7 +2284,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C3">
         <v>46.791699999999999</v>
@@ -2327,7 +2317,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C4">
         <v>49.373100000000001</v>
@@ -2360,7 +2350,7 @@
         <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5">
         <v>50.525100000000002</v>
@@ -2393,7 +2383,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C6">
         <v>48.524700000000003</v>
@@ -2426,7 +2416,7 @@
         <v>21</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>48.483899999999998</v>
@@ -2459,7 +2449,7 @@
         <v>21</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8">
         <v>47.264600000000002</v>
@@ -2492,7 +2482,7 @@
         <v>21</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>48.396299999999997</v>
@@ -2525,7 +2515,7 @@
         <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10">
         <v>48.411000000000001</v>
@@ -2558,7 +2548,7 @@
         <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C11">
         <v>45.2789</v>
@@ -2591,7 +2581,7 @@
         <v>21</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12">
         <v>46.311799999999998</v>
@@ -2624,7 +2614,7 @@
         <v>21</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>48.277200000000001</v>
@@ -2657,7 +2647,7 @@
         <v>21</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <v>51.385100000000001</v>
@@ -2690,7 +2680,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15">
         <v>49.022599999999997</v>
@@ -2723,7 +2713,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C16">
         <v>45.796500000000002</v>
@@ -2756,7 +2746,7 @@
         <v>21</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C17">
         <v>50.328800000000001</v>
@@ -2789,7 +2779,7 @@
         <v>19</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C18">
         <v>48.096200000000003</v>
@@ -2822,7 +2812,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C19">
         <v>48.282299999999999</v>
@@ -2855,7 +2845,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C20">
         <v>47.867100000000001</v>
@@ -2888,7 +2878,7 @@
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>48.981400000000001</v>
@@ -2921,7 +2911,7 @@
         <v>19</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C22">
         <v>45.036999999999999</v>
@@ -2954,7 +2944,7 @@
         <v>19</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C23">
         <v>50.251800000000003</v>
@@ -2987,7 +2977,7 @@
         <v>19</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C24">
         <v>49.472200000000001</v>
@@ -3020,7 +3010,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C25">
         <v>45.891599999999997</v>
@@ -3053,7 +3043,7 @@
         <v>19</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C26">
         <v>48.404800000000002</v>
@@ -3086,7 +3076,7 @@
         <v>19</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C27">
         <v>48.390300000000003</v>
@@ -3119,7 +3109,7 @@
         <v>19</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C28">
         <v>49.017600000000002</v>
@@ -3152,7 +3142,7 @@
         <v>19</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C29">
         <v>48.52</v>
@@ -3185,7 +3175,7 @@
         <v>19</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C30">
         <v>48.4788</v>
@@ -3218,7 +3208,7 @@
         <v>19</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C31">
         <v>48.093200000000003</v>
@@ -3251,7 +3241,7 @@
         <v>19</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C32">
         <v>48.274500000000003</v>
@@ -3284,7 +3274,7 @@
         <v>19</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C33">
         <v>46.786999999999999</v>
@@ -3317,7 +3307,7 @@
         <v>19</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C34">
         <v>50.325200000000002</v>
@@ -3350,7 +3340,7 @@
         <v>13</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C35">
         <v>47.261699999999998</v>
@@ -3383,7 +3373,7 @@
         <v>13</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C36">
         <v>50.521000000000001</v>
@@ -3416,7 +3406,7 @@
         <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C37">
         <v>46.308500000000002</v>
@@ -3449,7 +3439,7 @@
         <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C38">
         <v>51.381700000000002</v>
@@ -3482,7 +3472,7 @@
         <v>13</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C39">
         <v>45.277299999999997</v>
@@ -3515,7 +3505,7 @@
         <v>13</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C40">
         <v>49.371200000000002</v>
@@ -3548,7 +3538,7 @@
         <v>13</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C41">
         <v>48.4084</v>
@@ -3581,7 +3571,7 @@
         <v>13</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C42">
         <v>45.793799999999997</v>
@@ -3614,7 +3604,7 @@
         <v>13</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C43">
         <v>49.469700000000003</v>
@@ -3647,7 +3637,7 @@
         <v>13</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C44">
         <v>48.2791</v>
@@ -3680,7 +3670,7 @@
         <v>13</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C45">
         <v>46.788899999999998</v>
@@ -3713,7 +3703,7 @@
         <v>13</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C46">
         <v>47.863700000000001</v>
@@ -3746,7 +3736,7 @@
         <v>13</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C47">
         <v>48.2746</v>
@@ -3779,7 +3769,7 @@
         <v>13</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C48">
         <v>48.522300000000001</v>
@@ -3812,7 +3802,7 @@
         <v>13</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C49">
         <v>49.020299999999999</v>
@@ -3845,7 +3835,7 @@
         <v>13</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C50">
         <v>45.888599999999997</v>
@@ -3878,7 +3868,7 @@
         <v>12</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C51">
         <v>48.394300000000001</v>
@@ -3911,7 +3901,7 @@
         <v>12</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C52">
         <v>45.033999999999999</v>
@@ -3944,7 +3934,7 @@
         <v>12</v>
       </c>
       <c r="B53" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C53">
         <v>48.978200000000001</v>
@@ -3977,7 +3967,7 @@
         <v>12</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C54">
         <v>48.093899999999998</v>
@@ -4010,7 +4000,7 @@
         <v>12</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C55">
         <v>50.2485</v>
@@ -4043,7 +4033,7 @@
         <v>12</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C56">
         <v>48.401200000000003</v>
@@ -4076,7 +4066,7 @@
         <v>12</v>
       </c>
       <c r="B57" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C57">
         <v>48.4801</v>
@@ -4109,7 +4099,7 @@
         <v>12</v>
       </c>
       <c r="B58" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C58">
         <v>50.326599999999999</v>
@@ -4142,7 +4132,7 @@
         <v>12</v>
       </c>
       <c r="B59" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C59">
         <v>48.516500000000001</v>
@@ -4175,7 +4165,7 @@
         <v>12</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C60">
         <v>46.786299999999997</v>
@@ -4208,7 +4198,7 @@
         <v>12</v>
       </c>
       <c r="B61" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C61">
         <v>50.519599999999997</v>
@@ -4241,7 +4231,7 @@
         <v>12</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C62">
         <v>47.862699999999997</v>
@@ -4274,7 +4264,7 @@
         <v>12</v>
       </c>
       <c r="B63" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C63">
         <v>45.275399999999998</v>
@@ -4307,7 +4297,7 @@
         <v>12</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C64">
         <v>48.279200000000003</v>
@@ -4345,21 +4335,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8D6981C-AEB7-44A4-86BD-18E2FD352BF1}">
-  <dimension ref="A1:G63"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17:D33"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4367,1444 +4356,1255 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>208</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="B2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E2">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="F2">
+        <v>1.0725677830940077</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D3">
+        <v>1.3</v>
+      </c>
+      <c r="E3">
+        <v>6.4</v>
+      </c>
+      <c r="F3">
+        <v>1.0139846209012042</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" t="s">
+        <v>207</v>
+      </c>
+      <c r="D4">
+        <v>2.1999999999999997</v>
+      </c>
+      <c r="E4">
+        <v>18.099999999999998</v>
+      </c>
+      <c r="F4">
+        <v>1.4975874426891762</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D5">
+        <v>1.5</v>
+      </c>
+      <c r="E5">
+        <v>9.5</v>
+      </c>
+      <c r="F5">
+        <v>1.1940298507463143</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>196</v>
+      </c>
+      <c r="C6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D6">
+        <v>2.1</v>
+      </c>
+      <c r="E6">
+        <v>19.3</v>
+      </c>
+      <c r="F6">
+        <v>1.4036411284719206</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>197</v>
+      </c>
+      <c r="C7" t="s">
+        <v>207</v>
+      </c>
+      <c r="D7">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E7">
+        <v>12.8</v>
+      </c>
+      <c r="F7">
+        <v>1.1207417859302224</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" t="s">
+        <v>207</v>
+      </c>
+      <c r="D8">
+        <v>2.1</v>
+      </c>
+      <c r="E8">
+        <v>19.400000000000002</v>
+      </c>
+      <c r="F8">
+        <v>1.3387432737372382</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C9" t="s">
+        <v>207</v>
+      </c>
+      <c r="D9">
+        <v>1.2</v>
+      </c>
+      <c r="E9">
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="F9">
+        <v>1.1290257076716552</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>199</v>
+      </c>
+      <c r="C10" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E10">
+        <v>8.1</v>
+      </c>
+      <c r="F10">
+        <v>1.1150722915428846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>200</v>
+      </c>
+      <c r="C11" t="s">
+        <v>207</v>
+      </c>
+      <c r="D11">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E11">
+        <v>8</v>
+      </c>
+      <c r="F11">
+        <v>1.1432200698634631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>201</v>
+      </c>
+      <c r="C12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D12">
+        <v>1.3</v>
+      </c>
+      <c r="E12">
+        <v>7.5</v>
+      </c>
+      <c r="F12">
+        <v>0.96404477154247226</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>202</v>
+      </c>
+      <c r="C13" t="s">
+        <v>207</v>
+      </c>
+      <c r="D13">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E13">
+        <v>15.1</v>
+      </c>
+      <c r="F13">
+        <v>1.1088122451439102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
+        <v>203</v>
+      </c>
+      <c r="C14" t="s">
+        <v>207</v>
+      </c>
+      <c r="D14">
+        <v>1.3</v>
+      </c>
+      <c r="E14">
+        <v>5.5</v>
+      </c>
+      <c r="F14">
+        <v>0.96709065212999135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>204</v>
+      </c>
+      <c r="C15" t="s">
+        <v>207</v>
+      </c>
+      <c r="D15">
+        <v>1.4000000000000001</v>
+      </c>
+      <c r="E15">
+        <v>10.4</v>
+      </c>
+      <c r="F15">
+        <v>0.9434936102566972</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" t="s">
+        <v>205</v>
+      </c>
+      <c r="C16" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16">
+        <v>1.6</v>
+      </c>
+      <c r="E16">
+        <v>9.9</v>
+      </c>
+      <c r="F16">
+        <v>0.88497347081797073</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B17" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" t="s">
+        <v>209</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>5.3</v>
+      </c>
+      <c r="F17">
+        <v>0.81340293796296781</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B18" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E18">
+        <v>14.099999999999998</v>
+      </c>
+      <c r="F18">
+        <v>1.5847702581481711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B19" t="s">
+        <v>177</v>
+      </c>
+      <c r="C19" t="s">
+        <v>209</v>
+      </c>
+      <c r="D19">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E19">
+        <v>6.9</v>
+      </c>
+      <c r="F19">
+        <v>1.4055778823434615</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B20" t="s">
+        <v>178</v>
+      </c>
+      <c r="C20" t="s">
+        <v>209</v>
+      </c>
+      <c r="D20">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="E20">
+        <v>12.5</v>
+      </c>
+      <c r="F20">
+        <v>1.4157066363784025</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B21" t="s">
+        <v>179</v>
+      </c>
+      <c r="C21" t="s">
+        <v>209</v>
+      </c>
+      <c r="D21">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E21">
+        <v>15.2</v>
+      </c>
+      <c r="F21">
+        <v>1.5385537594660654</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B22" t="s">
+        <v>180</v>
+      </c>
+      <c r="C22" t="s">
+        <v>209</v>
+      </c>
+      <c r="D22">
+        <v>1.5</v>
+      </c>
+      <c r="E22">
+        <v>8.4</v>
+      </c>
+      <c r="F22">
+        <v>1.3870404258859685</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B23" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" t="s">
+        <v>209</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>4.8</v>
+      </c>
+      <c r="F23">
+        <v>1.2621985644004212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" t="s">
+        <v>209</v>
+      </c>
+      <c r="D24">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E24">
+        <v>18.099999999999998</v>
+      </c>
+      <c r="F24">
+        <v>1.4547500401865001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" t="s">
+        <v>183</v>
+      </c>
+      <c r="C25" t="s">
+        <v>209</v>
+      </c>
+      <c r="D25">
+        <v>1.9</v>
+      </c>
+      <c r="E25">
+        <v>14.099999999999998</v>
+      </c>
+      <c r="F25">
+        <v>1.4433231635765966</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B26" t="s">
+        <v>184</v>
+      </c>
+      <c r="C26" t="s">
+        <v>209</v>
+      </c>
+      <c r="D26">
+        <v>1.5</v>
+      </c>
+      <c r="E26">
+        <v>11.700000000000001</v>
+      </c>
+      <c r="F26">
+        <v>1.1850316076184055</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" t="s">
+        <v>185</v>
+      </c>
+      <c r="C27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D27">
+        <v>1.3</v>
+      </c>
+      <c r="E27">
+        <v>6.9</v>
+      </c>
+      <c r="F27">
+        <v>1.0571035363105965</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C28" t="s">
+        <v>209</v>
+      </c>
+      <c r="D28">
+        <v>2.5</v>
+      </c>
+      <c r="E28">
+        <v>24.099999999999998</v>
+      </c>
+      <c r="F28">
+        <v>1.3559965414706319</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" t="s">
+        <v>187</v>
+      </c>
+      <c r="C29" t="s">
+        <v>209</v>
+      </c>
+      <c r="D29">
+        <v>2.1</v>
+      </c>
+      <c r="E29">
+        <v>15.7</v>
+      </c>
+      <c r="F29">
+        <v>1.3585746102449157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B30" t="s">
+        <v>188</v>
+      </c>
+      <c r="C30" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E30">
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="F30">
+        <v>0.96209737227144732</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B31" t="s">
+        <v>189</v>
+      </c>
+      <c r="C31" t="s">
+        <v>209</v>
+      </c>
+      <c r="D31">
+        <v>2.5</v>
+      </c>
+      <c r="E31">
+        <v>20.5</v>
+      </c>
+      <c r="F31">
+        <v>1.2182943878569996</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B32" t="s">
+        <v>190</v>
+      </c>
+      <c r="C32" t="s">
+        <v>209</v>
+      </c>
+      <c r="D32">
+        <v>3.9</v>
+      </c>
+      <c r="E32">
+        <v>40.699999999999996</v>
+      </c>
+      <c r="F32">
+        <v>1.5403109146104272</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B33" t="s">
+        <v>191</v>
+      </c>
+      <c r="C33" t="s">
+        <v>209</v>
+      </c>
+      <c r="D33">
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="E33">
+        <v>73</v>
+      </c>
+      <c r="F33">
+        <v>2.2696744627054115</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" t="s">
+        <v>159</v>
+      </c>
+      <c r="C34" t="s">
+        <v>207</v>
+      </c>
+      <c r="D34">
+        <v>2</v>
+      </c>
+      <c r="E34">
+        <v>18.2</v>
+      </c>
+      <c r="F34">
+        <v>1.6295437277561942</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B35" t="s">
+        <v>160</v>
+      </c>
+      <c r="C35" t="s">
+        <v>207</v>
+      </c>
+      <c r="D35">
+        <v>1.2</v>
+      </c>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>1.2906052699714838</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" t="s">
+        <v>161</v>
+      </c>
+      <c r="C36" t="s">
+        <v>207</v>
+      </c>
+      <c r="D36">
+        <v>1.2</v>
+      </c>
+      <c r="E36">
+        <v>5.5</v>
+      </c>
+      <c r="F36">
+        <v>1.1968928344959053</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C37" t="s">
+        <v>207</v>
+      </c>
+      <c r="D37">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E37">
+        <v>7.6</v>
+      </c>
+      <c r="F37">
+        <v>1.1836470873395315</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B38" t="s">
+        <v>163</v>
+      </c>
+      <c r="C38" t="s">
+        <v>207</v>
+      </c>
+      <c r="D38">
+        <v>1.7000000000000002</v>
+      </c>
+      <c r="E38">
+        <v>12.9</v>
+      </c>
+      <c r="F38">
+        <v>1.2619372442018912</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" t="s">
+        <v>207</v>
+      </c>
+      <c r="D39">
+        <v>2</v>
+      </c>
+      <c r="E39">
+        <v>17.100000000000001</v>
+      </c>
+      <c r="F39">
+        <v>1.4508683227083137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B40" t="s">
+        <v>165</v>
+      </c>
+      <c r="C40" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40">
+        <v>1.2</v>
+      </c>
+      <c r="E40">
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="F40">
+        <v>1.1063183960379985</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B41" t="s">
+        <v>166</v>
+      </c>
+      <c r="C41" t="s">
+        <v>207</v>
+      </c>
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D2" t="s">
-        <v>208</v>
-      </c>
-      <c r="E2">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F2">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="G2">
-        <v>1.0725677830940077</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>195</v>
-      </c>
-      <c r="C3" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="F41">
+        <v>1.0620109821591162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B42" t="s">
+        <v>167</v>
+      </c>
+      <c r="C42" t="s">
+        <v>207</v>
+      </c>
+      <c r="D42">
+        <v>0.8</v>
+      </c>
+      <c r="E42">
+        <v>5.8999999999999995</v>
+      </c>
+      <c r="F42">
+        <v>1.0085241860943377</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B43" t="s">
+        <v>168</v>
+      </c>
+      <c r="C43" t="s">
+        <v>207</v>
+      </c>
+      <c r="D43">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E43">
+        <v>13.3</v>
+      </c>
+      <c r="F43">
+        <v>1.1914910891893342</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B44" t="s">
+        <v>169</v>
+      </c>
+      <c r="C44" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44">
+        <v>2.4</v>
+      </c>
+      <c r="E44">
+        <v>24.3</v>
+      </c>
+      <c r="F44">
+        <v>1.3626855669056974</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B45" t="s">
+        <v>170</v>
+      </c>
+      <c r="C45" t="s">
+        <v>207</v>
+      </c>
+      <c r="D45">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="E45">
+        <v>19.3</v>
+      </c>
+      <c r="F45">
+        <v>1.2781186094069528</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B46" t="s">
+        <v>171</v>
+      </c>
+      <c r="C46" t="s">
+        <v>207</v>
+      </c>
+      <c r="D46">
+        <v>3.2</v>
+      </c>
+      <c r="E46">
+        <v>32.9</v>
+      </c>
+      <c r="F46">
+        <v>1.5018249267037356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B47" t="s">
+        <v>172</v>
+      </c>
+      <c r="C47" t="s">
+        <v>207</v>
+      </c>
+      <c r="D47">
+        <v>2.9000000000000004</v>
+      </c>
+      <c r="E47">
+        <v>28.299999999999997</v>
+      </c>
+      <c r="F47">
+        <v>1.3953768118846441</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A48" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B48" t="s">
+        <v>173</v>
+      </c>
+      <c r="C48" t="s">
+        <v>207</v>
+      </c>
+      <c r="D48">
+        <v>2</v>
+      </c>
+      <c r="E48">
+        <v>16.8</v>
+      </c>
+      <c r="F48">
+        <v>1.1747018141725649</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A49" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="B49" t="s">
+        <v>174</v>
+      </c>
+      <c r="C49" t="s">
+        <v>207</v>
+      </c>
+      <c r="D49">
+        <v>1.5</v>
+      </c>
+      <c r="E49">
+        <v>9.5</v>
+      </c>
+      <c r="F49">
+        <v>1.0611963314666508</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" t="s">
         <v>209</v>
       </c>
-      <c r="E3">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F3">
-        <v>6.4000000000000001E-2</v>
-      </c>
-      <c r="G3">
-        <v>1.0139846209012042</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C4" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D4" t="s">
-        <v>208</v>
-      </c>
-      <c r="E4">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="F4">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="G4">
-        <v>1.4975874426891762</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>197</v>
-      </c>
-      <c r="C5" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D5" t="s">
-        <v>208</v>
-      </c>
-      <c r="E5">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F5">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="G5">
-        <v>1.1940298507463143</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>198</v>
-      </c>
-      <c r="C6" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="D50">
+        <v>1.7999999999999998</v>
+      </c>
+      <c r="E50">
+        <v>15</v>
+      </c>
+      <c r="F50">
+        <v>1.1858897182758199</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B51" t="s">
+        <v>146</v>
+      </c>
+      <c r="C51" t="s">
         <v>209</v>
       </c>
-      <c r="E6">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="F6">
-        <v>0.193</v>
-      </c>
-      <c r="G6">
-        <v>1.4036411284719206</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>199</v>
-      </c>
-      <c r="C7" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D7" t="s">
-        <v>208</v>
-      </c>
-      <c r="E7">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.128</v>
-      </c>
-      <c r="G7">
-        <v>1.1207417859302224</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>200</v>
-      </c>
-      <c r="C8" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="D51">
+        <v>1</v>
+      </c>
+      <c r="E51">
+        <v>5.2</v>
+      </c>
+      <c r="F51">
+        <v>0.98017285205899973</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s">
+        <v>147</v>
+      </c>
+      <c r="C52" t="s">
         <v>209</v>
       </c>
-      <c r="E8">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="F8">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="G8">
-        <v>1.3387432737372382</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C9" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D9" t="s">
-        <v>208</v>
-      </c>
-      <c r="E9">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F9">
-        <v>6.8000000000000005E-2</v>
-      </c>
-      <c r="G9">
-        <v>1.1290257076716552</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>201</v>
-      </c>
-      <c r="C10" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D10" t="s">
-        <v>208</v>
-      </c>
-      <c r="E10">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F10">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="G10">
-        <v>1.1150722915428846</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>202</v>
-      </c>
-      <c r="C11" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="F52">
+        <v>0.99173887575987663</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B53" t="s">
+        <v>148</v>
+      </c>
+      <c r="C53" t="s">
         <v>209</v>
       </c>
-      <c r="E11">
-        <v>1.4E-2</v>
-      </c>
-      <c r="F11">
-        <v>0.08</v>
-      </c>
-      <c r="G11">
-        <v>1.1432200698634631</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>203</v>
-      </c>
-      <c r="C12" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D12" t="s">
-        <v>208</v>
-      </c>
-      <c r="E12">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F12">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="G12">
-        <v>0.96404477154247226</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>204</v>
-      </c>
-      <c r="C13" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D13" t="s">
+      <c r="D53">
+        <v>1</v>
+      </c>
+      <c r="E53">
+        <v>5.8000000000000007</v>
+      </c>
+      <c r="F53">
+        <v>0.97505484683517096</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B54" t="s">
+        <v>149</v>
+      </c>
+      <c r="C54" t="s">
         <v>209</v>
       </c>
-      <c r="E13">
-        <v>1.4E-2</v>
-      </c>
-      <c r="F13">
-        <v>0.151</v>
-      </c>
-      <c r="G13">
-        <v>1.1088122451439102</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>205</v>
-      </c>
-      <c r="C14" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D14" t="s">
-        <v>208</v>
-      </c>
-      <c r="E14">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F14">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G14">
-        <v>0.96709065212999135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" t="s">
-        <v>206</v>
-      </c>
-      <c r="C15" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D15" t="s">
+      <c r="D54">
+        <v>1.6</v>
+      </c>
+      <c r="E54">
+        <v>12.7</v>
+      </c>
+      <c r="F54">
+        <v>1.1571899670231554</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B55" t="s">
+        <v>150</v>
+      </c>
+      <c r="C55" t="s">
         <v>209</v>
       </c>
-      <c r="E15">
-        <v>1.4E-2</v>
-      </c>
-      <c r="F15">
-        <v>0.104</v>
-      </c>
-      <c r="G15">
-        <v>0.9434936102566972</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" t="s">
-        <v>207</v>
-      </c>
-      <c r="C16" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D16" t="s">
-        <v>208</v>
-      </c>
-      <c r="E16">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F16">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="G16">
-        <v>0.88497347081797073</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="D55">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E55">
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="F55">
+        <v>1.0378827192527169</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C17" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D17" t="s">
-        <v>212</v>
-      </c>
-      <c r="E17">
-        <v>0.01</v>
-      </c>
-      <c r="F17">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="G17">
-        <v>0.81340293796296781</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="B56" t="s">
+        <v>151</v>
+      </c>
+      <c r="C56" t="s">
+        <v>209</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F56">
+        <v>0.93732400032192975</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B18" t="s">
-        <v>178</v>
-      </c>
-      <c r="C18" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D18" t="s">
-        <v>212</v>
-      </c>
-      <c r="E18">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F18">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="G18">
-        <v>1.5847702581481711</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="B57" t="s">
+        <v>152</v>
+      </c>
+      <c r="C57" t="s">
+        <v>209</v>
+      </c>
+      <c r="D57">
+        <v>1.2</v>
+      </c>
+      <c r="E57">
+        <v>7.3999999999999995</v>
+      </c>
+      <c r="F57">
+        <v>0.99259555733436244</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C19" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D19" t="s">
-        <v>212</v>
-      </c>
-      <c r="E19">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F19">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="G19">
-        <v>1.4055778823434615</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="B58" t="s">
+        <v>153</v>
+      </c>
+      <c r="C58" t="s">
+        <v>209</v>
+      </c>
+      <c r="D58">
+        <v>1.3</v>
+      </c>
+      <c r="E58">
+        <v>7.3</v>
+      </c>
+      <c r="F58">
+        <v>0.84993200543950242</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B20" t="s">
-        <v>180</v>
-      </c>
-      <c r="C20" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D20" t="s">
-        <v>212</v>
-      </c>
-      <c r="E20">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F20">
-        <v>0.125</v>
-      </c>
-      <c r="G20">
-        <v>1.4157066363784025</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
+      <c r="B59" t="s">
+        <v>154</v>
+      </c>
+      <c r="C59" t="s">
+        <v>209</v>
+      </c>
+      <c r="D59">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="E59">
+        <v>5</v>
+      </c>
+      <c r="F59">
+        <v>0.78015481197041447</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B21" t="s">
-        <v>181</v>
-      </c>
-      <c r="C21" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D21" t="s">
-        <v>212</v>
-      </c>
-      <c r="E21">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F21">
-        <v>0.152</v>
-      </c>
-      <c r="G21">
-        <v>1.5385537594660654</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="3" t="s">
+      <c r="B60" t="s">
+        <v>155</v>
+      </c>
+      <c r="C60" t="s">
+        <v>209</v>
+      </c>
+      <c r="D60">
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="E60">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="F60">
+        <v>0.80383273864415705</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C22" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D22" t="s">
-        <v>212</v>
-      </c>
-      <c r="E22">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F22">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="G22">
-        <v>1.3870404258859685</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="3" t="s">
+      <c r="B61" t="s">
+        <v>156</v>
+      </c>
+      <c r="C61" t="s">
+        <v>209</v>
+      </c>
+      <c r="D61">
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="E61">
+        <v>4.3</v>
+      </c>
+      <c r="F61">
+        <v>0.67575721008808665</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B23" t="s">
-        <v>183</v>
-      </c>
-      <c r="C23" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D23" t="s">
-        <v>212</v>
-      </c>
-      <c r="E23">
-        <v>0.01</v>
-      </c>
-      <c r="F23">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="G23">
-        <v>1.2621985644004212</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
+      <c r="B62" t="s">
+        <v>157</v>
+      </c>
+      <c r="C62" t="s">
+        <v>209</v>
+      </c>
+      <c r="D62">
+        <v>0.8</v>
+      </c>
+      <c r="E62">
+        <v>7.0000000000000009</v>
+      </c>
+      <c r="F62">
+        <v>0.66775936380746725</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="B24" t="s">
-        <v>184</v>
-      </c>
-      <c r="C24" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D24" t="s">
-        <v>212</v>
-      </c>
-      <c r="E24">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F24">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="G24">
-        <v>1.4547500401865001</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" t="s">
-        <v>185</v>
-      </c>
-      <c r="C25" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D25" t="s">
-        <v>212</v>
-      </c>
-      <c r="E25">
-        <v>1.9E-2</v>
-      </c>
-      <c r="F25">
-        <v>0.14099999999999999</v>
-      </c>
-      <c r="G25">
-        <v>1.4433231635765966</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B26" t="s">
-        <v>186</v>
-      </c>
-      <c r="C26" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D26" t="s">
-        <v>212</v>
-      </c>
-      <c r="E26">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F26">
-        <v>0.11700000000000001</v>
-      </c>
-      <c r="G26">
-        <v>1.1850316076184055</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B27" t="s">
-        <v>187</v>
-      </c>
-      <c r="C27" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D27" t="s">
-        <v>212</v>
-      </c>
-      <c r="E27">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F27">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="G27">
-        <v>1.0571035363105965</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B28" t="s">
-        <v>188</v>
-      </c>
-      <c r="C28" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D28" t="s">
-        <v>212</v>
-      </c>
-      <c r="E28">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F28">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="G28">
-        <v>1.3559965414706319</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B29" t="s">
-        <v>189</v>
-      </c>
-      <c r="C29" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D29" t="s">
-        <v>212</v>
-      </c>
-      <c r="E29">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="F29">
-        <v>0.157</v>
-      </c>
-      <c r="G29">
-        <v>1.3585746102449157</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B30" t="s">
-        <v>190</v>
-      </c>
-      <c r="C30" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D30" t="s">
-        <v>212</v>
-      </c>
-      <c r="E30">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F30">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="G30">
-        <v>0.96209737227144732</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B31" t="s">
-        <v>191</v>
-      </c>
-      <c r="C31" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D31" t="s">
-        <v>212</v>
-      </c>
-      <c r="E31">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F31">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="G31">
-        <v>1.2182943878569996</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B32" t="s">
-        <v>192</v>
-      </c>
-      <c r="C32" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D32" t="s">
-        <v>212</v>
-      </c>
-      <c r="E32">
-        <v>3.9E-2</v>
-      </c>
-      <c r="F32">
-        <v>0.40699999999999997</v>
-      </c>
-      <c r="G32">
-        <v>1.5403109146104272</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>144</v>
-      </c>
-      <c r="B33" t="s">
-        <v>193</v>
-      </c>
-      <c r="C33" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D33" t="s">
-        <v>212</v>
-      </c>
-      <c r="E33">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="F33">
-        <v>0.73</v>
-      </c>
-      <c r="G33">
-        <v>2.2696744627054115</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B34" t="s">
-        <v>161</v>
-      </c>
-      <c r="C34" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D34" t="s">
-        <v>208</v>
-      </c>
-      <c r="E34">
-        <v>0.02</v>
-      </c>
-      <c r="F34">
-        <v>0.182</v>
-      </c>
-      <c r="G34">
-        <v>1.6295437277561942</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B35" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="B63" t="s">
+        <v>158</v>
+      </c>
+      <c r="C63" t="s">
         <v>209</v>
       </c>
-      <c r="E35">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F35">
-        <v>0.08</v>
-      </c>
-      <c r="G35">
-        <v>1.2906052699714838</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B36" t="s">
-        <v>163</v>
-      </c>
-      <c r="C36" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D36" t="s">
-        <v>208</v>
-      </c>
-      <c r="E36">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F36">
-        <v>5.5E-2</v>
-      </c>
-      <c r="G36">
-        <v>1.1968928344959053</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B37" t="s">
-        <v>164</v>
-      </c>
-      <c r="C37" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D37" t="s">
-        <v>209</v>
-      </c>
-      <c r="E37">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F37">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="G37">
-        <v>1.1836470873395315</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B38" t="s">
-        <v>165</v>
-      </c>
-      <c r="C38" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D38" t="s">
-        <v>209</v>
-      </c>
-      <c r="E38">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="F38">
-        <v>0.129</v>
-      </c>
-      <c r="G38">
-        <v>1.2619372442018912</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B39" t="s">
-        <v>166</v>
-      </c>
-      <c r="C39" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D39" t="s">
-        <v>208</v>
-      </c>
-      <c r="E39">
-        <v>0.02</v>
-      </c>
-      <c r="F39">
-        <v>0.17100000000000001</v>
-      </c>
-      <c r="G39">
-        <v>1.4508683227083137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A40" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B40" t="s">
-        <v>167</v>
-      </c>
-      <c r="C40" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D40" t="s">
-        <v>209</v>
-      </c>
-      <c r="E40">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F40">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="G40">
-        <v>1.1063183960379985</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B41" t="s">
-        <v>168</v>
-      </c>
-      <c r="C41" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D41" t="s">
-        <v>208</v>
-      </c>
-      <c r="E41">
-        <v>0.01</v>
-      </c>
-      <c r="F41">
-        <v>0.06</v>
-      </c>
-      <c r="G41">
-        <v>1.0620109821591162</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A42" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B42" t="s">
-        <v>169</v>
-      </c>
-      <c r="C42" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D42" t="s">
-        <v>209</v>
-      </c>
-      <c r="E42">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="F42">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="G42">
-        <v>1.0085241860943377</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A43" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B43" t="s">
-        <v>170</v>
-      </c>
-      <c r="C43" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D43" t="s">
-        <v>208</v>
-      </c>
-      <c r="E43">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F43">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="G43">
-        <v>1.1914910891893342</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A44" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B44" t="s">
-        <v>171</v>
-      </c>
-      <c r="C44" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D44" t="s">
-        <v>209</v>
-      </c>
-      <c r="E44">
-        <v>2.4E-2</v>
-      </c>
-      <c r="F44">
-        <v>0.24299999999999999</v>
-      </c>
-      <c r="G44">
-        <v>1.3626855669056974</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A45" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B45" t="s">
-        <v>172</v>
-      </c>
-      <c r="C45" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D45" t="s">
-        <v>209</v>
-      </c>
-      <c r="E45">
-        <v>2.3E-2</v>
-      </c>
-      <c r="F45">
-        <v>0.193</v>
-      </c>
-      <c r="G45">
-        <v>1.2781186094069528</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A46" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B46" t="s">
-        <v>173</v>
-      </c>
-      <c r="C46" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D46" t="s">
-        <v>208</v>
-      </c>
-      <c r="E46">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="F46">
-        <v>0.32900000000000001</v>
-      </c>
-      <c r="G46">
-        <v>1.5018249267037356</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A47" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B47" t="s">
-        <v>174</v>
-      </c>
-      <c r="C47" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D47" t="s">
-        <v>209</v>
-      </c>
-      <c r="E47">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="F47">
-        <v>0.28299999999999997</v>
-      </c>
-      <c r="G47">
-        <v>1.3953768118846441</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A48" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B48" t="s">
-        <v>175</v>
-      </c>
-      <c r="C48" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D48" t="s">
-        <v>208</v>
-      </c>
-      <c r="E48">
-        <v>0.02</v>
-      </c>
-      <c r="F48">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="G48">
-        <v>1.1747018141725649</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A49" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B49" t="s">
-        <v>176</v>
-      </c>
-      <c r="C49" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D49" t="s">
-        <v>209</v>
-      </c>
-      <c r="E49">
-        <v>1.4999999999999999E-2</v>
-      </c>
-      <c r="F49">
-        <v>9.5000000000000001E-2</v>
-      </c>
-      <c r="G49">
-        <v>1.0611963314666508</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B50" t="s">
-        <v>147</v>
-      </c>
-      <c r="C50" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D50" t="s">
-        <v>210</v>
-      </c>
-      <c r="E50">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="F50">
-        <v>0.15</v>
-      </c>
-      <c r="G50">
-        <v>1.1858897182758199</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A51" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B51" t="s">
-        <v>148</v>
-      </c>
-      <c r="C51" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D51" t="s">
-        <v>210</v>
-      </c>
-      <c r="E51">
-        <v>0.01</v>
-      </c>
-      <c r="F51">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="G51">
-        <v>0.98017285205899973</v>
-      </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A52" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B52" t="s">
-        <v>149</v>
-      </c>
-      <c r="C52" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D52" t="s">
-        <v>210</v>
-      </c>
-      <c r="E52">
-        <v>0.01</v>
-      </c>
-      <c r="F52">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="G52">
-        <v>0.99173887575987663</v>
-      </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A53" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B53" t="s">
-        <v>150</v>
-      </c>
-      <c r="C53" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D53" t="s">
-        <v>210</v>
-      </c>
-      <c r="E53">
-        <v>0.01</v>
-      </c>
-      <c r="F53">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="G53">
-        <v>0.97505484683517096</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A54" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B54" t="s">
-        <v>151</v>
-      </c>
-      <c r="C54" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D54" t="s">
-        <v>210</v>
-      </c>
-      <c r="E54">
-        <v>1.6E-2</v>
-      </c>
-      <c r="F54">
-        <v>0.127</v>
-      </c>
-      <c r="G54">
-        <v>1.1571899670231554</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A55" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B55" t="s">
-        <v>152</v>
-      </c>
-      <c r="C55" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D55" t="s">
-        <v>210</v>
-      </c>
-      <c r="E55">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F55">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="G55">
-        <v>1.0378827192527169</v>
-      </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A56" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B56" t="s">
-        <v>153</v>
-      </c>
-      <c r="C56" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D56" t="s">
-        <v>210</v>
-      </c>
-      <c r="E56">
-        <v>0.01</v>
-      </c>
-      <c r="F56">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="G56">
-        <v>0.93732400032192975</v>
-      </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A57" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B57" t="s">
-        <v>154</v>
-      </c>
-      <c r="C57" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D57" t="s">
-        <v>210</v>
-      </c>
-      <c r="E57">
-        <v>1.2E-2</v>
-      </c>
-      <c r="F57">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="G57">
-        <v>0.99259555733436244</v>
-      </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A58" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B58" t="s">
-        <v>155</v>
-      </c>
-      <c r="C58" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D58" t="s">
-        <v>210</v>
-      </c>
-      <c r="E58">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="F58">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="G58">
-        <v>0.84993200543950242</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A59" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B59" t="s">
-        <v>156</v>
-      </c>
-      <c r="C59" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D59" t="s">
-        <v>210</v>
-      </c>
-      <c r="E59">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="F59">
-        <v>0.05</v>
-      </c>
-      <c r="G59">
-        <v>0.78015481197041447</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A60" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C60" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D60" t="s">
-        <v>210</v>
-      </c>
-      <c r="E60">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="F60">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="G60">
-        <v>0.80383273864415705</v>
-      </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A61" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B61" t="s">
-        <v>158</v>
-      </c>
-      <c r="C61" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D61" t="s">
-        <v>210</v>
-      </c>
-      <c r="E61">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="F61">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="G61">
-        <v>0.67575721008808665</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A62" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B62" t="s">
-        <v>159</v>
-      </c>
-      <c r="C62" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D62" t="s">
-        <v>210</v>
-      </c>
-      <c r="E62">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="F62">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="G62">
-        <v>0.66775936380746725</v>
-      </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A63" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="B63" t="s">
-        <v>160</v>
-      </c>
-      <c r="C63" s="7">
-        <v>44501</v>
-      </c>
-      <c r="D63" t="s">
-        <v>210</v>
+      <c r="D63">
+        <v>1.5</v>
       </c>
       <c r="E63">
-        <v>1.4999999999999999E-2</v>
+        <v>10.5</v>
       </c>
       <c r="F63">
-        <v>0.105</v>
-      </c>
-      <c r="G63">
         <v>0.73533819562407032</v>
       </c>
     </row>

</xml_diff>